<commit_message>
added latest XMAML codes
</commit_message>
<xml_diff>
--- a/get-discourse-datasets/TextClassification/sentences/csv/sentences_ocr_corrected_discourse_profiling_ar.xlsx
+++ b/get-discourse-datasets/TextClassification/sentences/csv/sentences_ocr_corrected_discourse_profiling_ar.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="247">
   <si>
     <t>Sentence_ar</t>
   </si>
@@ -25,19 +25,24 @@
     <t>Year</t>
   </si>
   <si>
-    <t>قاتل احدا ذاهبا الى الحرب وحريه القرار اللبناني محترمه  وفي معرض حديثه الوضع الخاص الجنوب اكد توينيان اللبنانيين ضد وجود المقاومه  الفلسطينيه ونحن متضامنون معهم انما الارض اللبنانيه مقدسه بالنسبه الينا تماما ارضهم مقدسه  بالنسبه اليهم ولسنا استعداد لنضيع اي شبر ارض المقاومه قضيتها المقدسه السباده اللبنانيه الكاهله  ارضنا وكهانكن نساعدهم تاكيد حريه القرار الفلسطيبني ننتظر ونريد ان تؤكد حريه  القرار اللبناني وراى الدوله المحترمه يجب ان تكون استراتيجيه  مدركه تتكيف مع الاحداث</t>
-  </si>
-  <si>
-    <t>صمود وتجمع الى الصمود وعي العباء يستطيع لبنان عموما وجنوبه خصوصا  ان يتحمله واعتقد ان الثوره الفلسطينيه والقوى الوطنيه يمكن ان تفرط قيد  شعره بهذا المعقل الحصين واضاف تحتاجه اسرائيل لذلك تدعو الى ان تترسخ وتنمو مقاومه  وطنيه لبنانبه شامله للخطر الصهيوني يتجدد الجنوب فتصبح المقاومه الفلسطينيه قوه دعم  لهويه الجنوب يبقى مجرد راقعه للثوره الفلسطينيه بكل مساهمه رسميه تريد ان  تدعم جنوبا مقاوما وطنيا قادرا الصمود وجه اسرائيل لان لا بديل للمواجهه الشامله للتعاطي قضيه الجنوب</t>
-  </si>
-  <si>
-    <t>القيادات نجاح الاجتماع تدعي اليه لجنه التوصل الى نيل الصعوبات تعترض تشكيل هيئه  الرقابه بتفاهم لبناني سوري فهذه الظروف يظهر فيها خطر قيام اسرائيل باعتداء الجنوب  وعلى المقاومه الفلسطينيه الصعب من غير المقبول تطبيق صلاحيات هيئه الرقابه بمنع الاسلحه  المقاومه ان السعوديه والكويت مستعدين لحضور اجتماع لجنه المتابعه يكن مجدي</t>
-  </si>
-  <si>
-    <t>ارضا وشعبا ويحقق التضامن اللبناني الفلسطيني ويكفل حمايه الثوره الفلسطينيه وتعزيز دورها النضالي  ضد العدو الصهبوني ناقش الجانب ان التهديدات الاسرائيليه للبنان والتي تاتي اطار اطماع اسرائيل الاراضي اللبنانيه  وتصفيه المقاومه الفلسطينيه وبالتالي تحقيق حلقه جديده مخططاتها العدو واكد الجانبان وقوفهما لبنان بكل  امكاناتهما لمواجهه المخططات الاسرائيليه اكدا انهما سيعملان تعزيز وحده القوتين الثوره وجمايه الجنوب  للصمود مواجهه العدوان الاسرائيلي</t>
-  </si>
-  <si>
-    <t>عدم الانسحاب الجنوب الا التاكد وصول رئيس للجمهوريه في لبنان مستعد  للدخول مثل المفاوضات والقبول بتوطين الفلسطينيين لبنان ضبط وجودهم المسلح وهذا  يمكن تحقيقه طريق اقامه دوله قويه قادره وسلطه مركزيه فاعله لذلك فان  تهديدات اسرائيل بضرب المقاومه الفلسطينيه بحجه انها تخرق وقف النار تسمح  بخرقه الجنوب مكان العالم تستهدف المقاومه بقدر تستهدف الجنوب نفسه تحقيقا لاهدافها  وهي تهديدات ستنفذها الوقت المناسب حاجاتها الخاصه</t>
+    <t>كاالا قاتل داري احدا ذاهيا الي الحرب وحريهالقرار اللبناني محترمه  ”وفي معرض حديثه ”الوضعالخاص الجنوب اكد توينيان اللبتانيين ضد وجودالمقاومه  الفلسطينيه ونصنمتضامتون معهم انما الارضاللبنانيه مقدسه بالمنسبه الينا تماماارضهم مقدسه  بالنسبه اليهمولسنا استعداد لنضيع اي شبرارضتاء المقاومهقضيتها المقدسه السبادهاللبنانيه الكاهله  ارضناء وكهانكن نساعدهم تاكيد حريه القرارالفلسطيبني ننتظر ونريد ان تؤكدحريه  القرار اللبناني وصابهلاخد قابن الجنابهوراي الدوله المحترمه يجبان تكون استرانيجيه  متدركهتتكيف هع الاحداتث
+  قاتل احدا ذاهبا الى الحرب وحريه القرار اللبناني محترمه  وفي معرض حديثه الوضع الخاص الجنوب اكد توينيان اللبنانيين ضد وجود المقاومه  الفلسطينيه ونحن متضامنون معهم انما الارض اللبنانيه مقدسه بالنسبه الينا تماما ارضهم مقدسه  بالنسبه اليهم ولسنا استعداد لنضيع اي شبر ارض المقاومه قضيتها المقدسه السباده اللبنانيه الكاهله  ارضنا وكهانكن نساعدهم تاكيد حريه القرار الفلسطيبني ننتظر ونريد ان تؤكد حريه  القرار اللبناني وراى الدوله المحترمه يجب ان تكون استراتيجيه  مدركه تتكيف مع الاحداث</t>
+  </si>
+  <si>
+    <t>صمودا مفيقياوتجمع الي الصمود وعيا تحجمالعباء يستطيع لبنان عموماوجنوبه خصوصا  ان يتحمنه واعتقدان الثوره الفلسطينيه والقويالوطنيه يمكن ان تفرط قيد  شعرهبهذا المعقل الحصينواضافتجتاحه اسرائيل لذلك تدعو الي انتترسخ وتتمو مقاومه  وطنيه لبنانبهسامي عيادشامله للخطر الصهيوني يتجددالجنوبء فتصبح المقاومهالفلسطينيه قوه دعم  لهويه الجنوبيبقي مجرد راقعه للتورهالفلسطينيه نرب بكلمساهمه رسميه تريد ان  تدعم جنوبامقاوما وطنيا قادرا الصمودوجهاسراشيل  لاندلا بديلالمواجهه الشامله للتعاطي قضيهالجنوب
+  صمود وتجمع الى الصمود وعي العباء يستطيع لبنان عموما وجنوبه خصوصا  ان يتحمله واعتقد ان الثوره الفلسطينيه والقوى الوطنيه يمكن ان تفرط قيد  شعره بهذا المعقل الحصين واضاف تحتاجه اسرائيل لذلك تدعو الى ان تترسخ وتنمو مقاومه  وطنيه لبنانبه شامله للخطر الصهيوني يتجدد الجنوب فتصبح المقاومه الفلسطينيه قوه دعم  لهويه الجنوب يبقى مجرد راقعه للثوره الفلسطينيه بكل مساهمه رسميه تريد ان  تدعم جنوبا مقاوما وطنيا قادرا الصمود وجه اسرائيل لان لا بديل للمواجهه الشامله للتعاطي قضيه الجنوب</t>
+  </si>
+  <si>
+    <t>القياداتنجاحلاجتماع تدعي اليد لجنهالتوصل الي ليل الصعوبات تعترض تشكيل هيكه  الرقابهبتفاهم لبناني سوري فهذه الظروف يظهرقيها خطرقيام اسرائيل باعتداء الجنوب  وعلي المقاومهالفلسطينيه الصعبء منغير المقبول تطبيقصلاحيات هيئه اللرقابه بمنع الاسلحه  المقاومه انالسعوديه والكويت مستعدتين لحضور اجتماع لجنهالمتابعه يكن مجديا
+  القيادات نجاح الاجتماع تدعي اليه لجنه التوصل الى نيل الصعوبات تعترض تشكيل هيئه  الرقابه بتفاهم لبناني سوري فهذه الظروف يظهر فيها خطر قيام اسرائيل باعتداء الجنوب  وعلى المقاومه الفلسطينيه الصعب من غير المقبول تطبيق صلاحيات هيئه الرقابه بمنع الاسلحه  المقاومه ان السعوديه والكويت مستعدين لحضور اجتماع لجنه المتابعه يكن مجدي</t>
+  </si>
+  <si>
+    <t>ارضا وشعباء ويحقق التلاضماللبناني الفلسطيني ويكفل حمايهالثوره الفلسطينيه وتعزيز دورهاالنضالي  ضد العدو الصهبونيناقش الجانبانالتهديدات الاسرائيليه للبنانوالتيتاتي اطار اطماع اسرائيلالاراضي اللبنانيه  وتصفيه المقاومهالفلسطينيه وبالتالي تحقيق حلقهجديده مخظطاتها العدواواكد الجانبان وقوفهما لبنانبكل  امكاناتهما لمواجمه المخططاتالاسرائيليه اكدا انههما سيعملانتعزيز وحده القوين الثورهوجماهيرما الجنوب  للصمودمواجهه العدوان الاسرائيليساناء وقاءكونا
+  ارضا وشعبا ويحقق التضامن اللبناني الفلسطيني ويكفل حمايه الثوره الفلسطينيه وتعزيز دورها النضالي  ضد العدو الصهبوني ناقش الجانب ان التهديدات الاسرائيليه للبنان والتي تاتي اطار اطماع اسرائيل الاراضي اللبنانيه  وتصفيه المقاومه الفلسطينيه وبالتالي تحقيق حلقه جديده مخططاتها العدو واكد الجانبان وقوفهما لبنان بكل  امكاناتهما لمواجهه المخططات الاسرائيليه اكدا انهما سيعملان تعزيز وحده القوتين الثوره وجمايه الجنوب  للصمود مواجهه العدوان الاسرائيلي</t>
+  </si>
+  <si>
+    <t>عدم الاتسحاب اللجنوب الا التاكد وصولرئيس للجمهوريه شي لبنان مستعد  للدخول مثلالمفاوضات والقبول بتوطين الفلسطينيين لبنان ضبطوجودهم المسلح وتدجيتهم وهذا  يمكن تحقيقه طريقاقامه دوله قويه قادره وسلطه مركزيه فاعلهلذلك فان  تهديدات اسرائيل بضرب المقاومه الفلسطينيهبحجه انها تخرق وقف النار تسمح  بخرقه الجنوبمكان العالم تستهدف المقاومه بقدرتستهدف الجنوب نفسه تحقيقا لاهدافها  وهي تهديداتستنفذها الوقت المناسباميل خوريحاجاتهاالخاصبه
+  عدم الانسحاب الجنوب الا التاكد وصول رئيس للجمهوريه في لبنان مستعد  للدخول مثل المفاوضات والقبول بتوطين الفلسطينيين لبنان ضبط وجودهم المسلح وهذا  يمكن تحقيقه طريق اقامه دوله قويه قادره وسلطه مركزيه فاعله لذلك فان  تهديدات اسرائيل بضرب المقاومه الفلسطينيه بحجه انها تخرق وقف النار تسمح  بخرقه الجنوب مكان العالم تستهدف المقاومه بقدر تستهدف الجنوب نفسه تحقيقا لاهدافها  وهي تهديدات ستنفذها الوقت المناسب حاجاتها الخاصه</t>
   </si>
   <si>
     <t>في ببروتالغربيه وقال عندما بدااتالمقاومه الفلسطينيه بالممارساتنالشاطئه وبالتجاوزات وقفناالمظلومين والان  نرقض مثلالتجاوزات ونرفضص عوده المقاومهالفلسطينيه الي كانت عليم قبلالاجتياح الاسراكيلي  للبنانواشاد بمقاومه الجنوبيين للاحتلالالاسرائيلي مشيرا الي انالمقاومه الجنوب اسلاميه لانقادتها  العلماء
@@ -600,6 +605,342 @@
   لتنو لله مسخصه الاتقماه تعلفه لمصمتقكعامضم اتهمته بالتعريض مجزره صبرا  وشاتيلا بيروت عام وهذه المحركه منشقه حزب العمل ولها ثلاثه مقاعد الكنيسه وذكرت  عريضتها ان شارون قال حينه انو سيغيب اسبوعين فقط وقد انهي شمادتهه قبل  بضعه ايام واثار غياب الوزير نقاشا حادا مجلس الوزراء الاسرائيلي الاحد الماضي ودعا  حاييم بارليف وزير الشرطه شارون المي السعوده اوالاستقائه بالمتمناه عدي ععاندع عنتمم  رعقسامه اه بثزنه قو نافغنالنه</t>
   </si>
   <si>
+    <t>رويتر غادرامس وزير الصناعه الاسرائيلي ارييلشارونء العشل اللممدبر لنفزوالاسرائيلي للبنان  تل ابيبطريقه الي نيويورك لمتابعهالدعوي اقامها مجله تايمالاميركيه مزودا شهاده  جديده قال انهاواقادت وزاره العدل ان رئيسالمحكمه العليا السابق اسحق  كاهانراس نجنه التحقيق الاسرائيليهمجزره صبرا وشاتيلا شهد بانزيرللدفاع المجله الاميركيهمطالبا  بتعويض مليون دولار لانهازعمت الملحق اشار الي انه ناقشضمساله الثار  اسره الجميل
+  رويترز غادر امس وزير الصناعه الاسرائيلي ارييل شارون والاسرائيلي للبنان  تل ابيب طريقه الى نيويورك لمتابعه الدعوى اقامها مجله تايم الاميركيه مزودا شهاده  جديده قال انها وافادت وزاره العدل ان رئيس المحكمه العليا السابق اسحق  كاهان راس لجنه التحقيق الاسرائيليه مجزره صبرا وشاتيلا شهد بان وزير للدفاع المجله الاميركيه مطالبا  بتعويض مليون دولار لانها زعمت الملحق اشار الى انه ناقش مساله الثار  اسره الجميل</t>
+  </si>
+  <si>
+    <t>واعتبرت الميئشه انشارون شومت نتيجه روايه نشرتهاالمجله مجزره مخيمي صبرا  وشاتيلابيروتوواصل المحلفون وهم سيداتورجلانء مداولاتهم الجانبينالاخرين لدعوي القدح بموجب قانونالولايات  المتحده وهما اذا كانتالروايه زائفه اذا كانت المجلهنشرتها وهي علم  بانها زائفه اواهملت بالتغاضي الحقيقه
+  واعتبرت الميئشه ان شارون شومت نتيجه روايه نشرتها المجله مجزره مخيمي صبرا  وشاتيلا بيروت وواصل المحلفون وهم سيدات ورجلان مداولاتهم الجانبين الاخرين لدعوى القدح بموجب قانون الولايات  المتحده وهما اذا كانت الروايه زائفه اذا كانت المجله نشرتها وهي علم  بانها زائفه او اهملت بالتغاضي الحقيقه</t>
+  </si>
+  <si>
+    <t>المحكمهخسر امس ارييل شارون وزيرالتجاره والصناعه الاسرائيلي كانوزيرا للدفاع وقوع  مجزره مخيميصبرا وشاتيلاء دعوي القدحاقامها مجله تايم الاميركيهنيويورك مطالبا بتعويضات  تقدر بمليون دولارء بعدما قررت هيئهالمحلفين المحكمه ان المجلهتتشر المقال  موضوع الدعوي سوءنيه
+  المحكمه خسر امس ارييل شارون وزير التجاره والصناعه الاسرائيلي كان وزيرا للدفاع وقوع  مجزره مخيمي صبرا وشاتيلا دعوى القدح اقامها مجله تايم الاميركيه نيويورك مطالبا بتعويضات  تقدر بمليون دولار بعدما قررت هيئه المحلفين المحكمه ان المجله تنشر المقال  موضوع الدعوى سوء نيه</t>
+  </si>
+  <si>
+    <t>القدس قال اسحق شاميروزير الخارجيه الاسرائيلي وزعيم تكتلليكود ان قرار  هيئه المحلفين اثبتان نشرته ثايم علاقه شارونبمجزره صبرا وشاتيلا يعدو  كونهتفسيرا اساس له
+  القدس قال اسحق شامير وزير الخارجيه الاسرائيلي وزعيم تكتل ليكود ان قرار  هيئه المحلفين اثبت ان نشرته تايم علاقه شارون بمجزره صبرا وشاتيلا يعدو  كونه تفسيرا اساس له</t>
+  </si>
+  <si>
+    <t>وسر انصار شارون اسرائيلبنجاح وزير الدفاع السابق غسليديه مجزره مخيمي  صبرا وشاتيلا
+  وسر انصار شارون اسرائيل بنجاح وزير الدفاع السابق غسل يديه مجزره مخيمي  صبرا وشاتيلا</t>
+  </si>
+  <si>
+    <t>بينماقال المئه انهم وقفواويشار الي ان شارون خسر الشهرالماضي دعواه  المجله اتهمتههبالتشجيع مجزره صبرا وشاتيلاءواعتبر المكه ان تطورالمحاكمه برا شارون  المسؤولياتحمله اياها تقرير كاهان شانالمجزره
+  بينما قال المئه انهم وقفوا ويشار الى ان شارون خسر الشهر الماضي دعواه  المجله اتهمته التشجيع مجزره صبرا وشاتيلا واعتبر ان تطور المحاكمه برا شارون  المسؤوليات حمله اياها تقرير كاهان شان المجزره</t>
+  </si>
+  <si>
+    <t>وتساعل الفرق جرائمالكتائب صبرا وشاتيلا وجرائمالبعث وحركه تشرين طرابلسوقال ايجهم  اكثر بغياء قتلواالناس ام اعتقلوهم ليحققواوردا المطالبين بتسليمالموقوفين الي الدوله  قال تسلمالمجرم الي ارسله الهنا وذكربمصير اوقفوا بتهمه ارتكابمجزره البحصاص  قبل اقل عامينسلموا الي الدوله ولم يعاقباحد منهم
+  وتسائل الفرق جرائم الكتائب صبرا وشاتيلا وجرائم البعث وحركه تشرين طرابلس وقال ايجهم  اكثر بغياء قتلوا الناس ام اعتقلوهم ليحققوا وردا المطالبين بتسليم الموقوفين الى الدوله  قال تسلم المجرم الى ارسله الينا وذكر بمصير اوقفوا بتهمه ارتكاب مجزره البحصاص  قبل اقل عامين سلموا الى الدوله ولم يعاقب احد منهم</t>
+  </si>
+  <si>
+    <t>تاتي الذكريوهنا نص البيانالثامنه لاستشهاد اتقائد المعلم كمالجنبلاط ومعركه تحرير  لبنانالاحتلال الاسرائيلي وعملائه وافرازاتهتبلغ ذروتها تصاعد العملياتالبظوليه لجبهه المقاومه الوطئيهاللبنائيه  وفي صمود جماهير الجنوبوالبقاع الغربي وراشيا وجه بربريهالصهاينه وهمجيتهمم والتي  تضاهيالجرائم المنازيه تشهد بذلك مجازرالزراريه ومعركه وبئر العبد وقبلهامجزره صبرا  وشاتيلا وغيرهاالجرائم تكشف مدي الحقدالمستيري للعدو الاسرائيلي ثارالهزيمته العسكريه والسياسيهواضطراره  الي الانسهاب قهدشرط رغم الخسائر الجسيمهيتكبدما
+  تاتي الذكرى وهنا نص البيان الثامنه لاستشهاد القائد المعلم كمال جنبلاط ومعركه تحرير  لبنان الاحتلال الاسرائيلي وعملائه وافرازاته تبلغ ذروتها تصاعد العمليات البطوليه لجبهه المقاومه الوطنيه اللبنانيه  وفي صمود جماهير الجنوب والبقاع الغربي وراشيا وجه بربريه الصهاينه وهمجيتهم والتي  تضاهي الجرائم المنازيه تشهد بذلك مجازر الزراريه ومعركه وبئر العبد وقبلها مجزره صبرا  وشاتيلا وغيرها الجرائم تكشف مدى الحقد المستشري للعدو الاسرائيلي ثار لهزيمته العسكريه والسياسيه واضطراره  الى الانسحاب شرط رغم الخسائر الجسيمه يتكبدها</t>
+  </si>
+  <si>
+    <t>نذكرهصبرا وشاتيلا المجزره خجلالعالم خجل المتريعون باسمناباسم الشرعيه تفغطيهالمؤامره استجدفت  الشعبالاعزل والابرياء والاطفال والنساءوالشهوخ
+  نذكره صبرا وشاتيلا المجزره خجل العالم خجل المتريعون باسمنا باسم الشرعيه تغطيه المؤامره استهدفت  الشعب الاعز والابرياء والاطفال والنساء والشيوخ</t>
+  </si>
+  <si>
+    <t>فا لمنمجيهسمير جعجع اعتبارا مجزره اهدنمرورا بالاجتياح الاسرائيلي رافقهمجازر صبرا  وشاتيلا وصولا اليقيادته حرب الجبل واخلاثه اسرائيلهادير القمر المحاصره وانتهاء  باعادهتركيزه بلاد جبيل ان المتتبع لكليري بوضوح الخط الاسرائيليالمتواصل المنهجيهتكون  بلفت ذروتها التحرك الاخيريقوده بالاشتراك رموز اخريقللخط نفسه
+  فالمنهجيه سمير جعجع اعتبارا مجزره اهدن مرورا بالاجتياح الاسرائيلي رافقه مجازر صبرا  وشاتيلا وصولا الى قيادته حرب الجبل واخلائه اسرائيل دير القمر المحاصره وانتهاء  باعاده تركيزه بلاد جبيل ان المتتبع لكل يري بوضوح الخط الاسرائيلي المتواصل المنهجيه تكون  بلغت ذروتها التحرك الاخير يقوده بالاشتراك رموز اخرى للخط نفسه</t>
+  </si>
+  <si>
+    <t>ونعلمايضا ان الخلافات اميركاواسرائيل تشمل شؤونا عده وانالسفير الاميركي روبرت  ديلون حذربعبارات تثير التباسمشاركه القوات اللبنانيه الي جانباسرائيل عملياتها لبنانيعرض  لاقصي الخطر القياده نفسهاوفي صدد مجزره صبرا وشاتيلا تعجدقيليب حبيب  للرئيسين صائب سلاموشقيق الوزان عدم حصولها
+  ونعلم ايضا ان الخلافات اميركا واسرائيل تشمل شؤونا عده وان السفير الاميركي روبرت  ديلون حذر بعبارات تثير التباس مشاركه القوات اللبنانيه الى جانب اسرائيل عملياتها لبنان يعرض  لاقصى الخطر القياده نفسها وفي صدد مجزره صبرا وشاتيلا تعجب فيليب حبيب  للرئيسين صائب سلام وشقيق الوزان عدم حصولها</t>
+  </si>
+  <si>
+    <t>وقد اعغترض السفيرواكد ان فرنسا تريد ان تحل اليهوممفهوما ينطلق  الثوره الفرنسيهوذكرته بدور فرتم القوهالمتعدده الجنسيه دخلت لوقفالانهيار الماروني وانسحبت  قبل وقوعمجزره صبرا وشاتيلا بساعات لتتمالفاجعه غياب الشهود
+  وقد اعترض السفير واكد ان فرنسا تريد ان تحل اليوم مفهوما ينطلق  الثوره الفرنسيه وذكرته بدور القوه المتعدده الجنسيه دخلت لوقف الانهيار الماروني وانسحبت  قبل وقوع مجزره صبرا وشاتيلا بساعات لتتم الفاجعه غياب الشهود</t>
+  </si>
+  <si>
+    <t>ايضا يمنع الجيشمواجمه الانتفاضه قامت ضدهومتعتر ممارسه حقه القراروحمل اركان  الانتفاضه ”واتهمهم بانجم مارسواجرائمهم ضد فرنجيه الشمال وضدشمعون وابنه الصقرا  وضدالمسيحي الاشرفيه وفي مكانوهم ارتكبوا مجزره صبراوشاتيلا
+  ايضا يمنع الجيش مواجهه الانتفاضه قامت ضده وتعتبر ممارسه حقه القرار وحمل اركان  الانتفاضه واتهمهم بانهم مارسوا جرائمهم ضد فرنجيه الشمال وضد شمعون وابنه الصقرا  وضد المسيحي الاشرفيه وفي مكان وهم ارتكبوا مجزره صبرا وشاتيلا</t>
+  </si>
+  <si>
+    <t>افتمل عمان اف يبغدادتتمه المنشور الصفحهجنوب لبنان وققا للنارالفلسطينيين واسرائيل  فتحولتحضيرا للفزو الاسرائكيلي للبنانحزيران ومحاوله لضرب الوجودالعسكري والسياسي لمنظمه التحريرالفلسطينيه  اضافه الي انها تحترمتعهداتها لحمايه المخيماتالفلسطينيه اثر الخروج لبنانوانتهي الامر  الي انسحاب اميركيمفاجيء للمجزره الصهيونيهالكتائبيه البشعه صبرا وشاتيلا
+  افتمل عمان في بغداد جنوب لبنان وقفا للنار الفلسطينيين واسرائيل  فتحول تحضيرا للغزو الاسرائيلي للبنان حزيران ومحاوله لضرب الوجود العسكري والسياسي لمنظمه التحرير الفلسطينيه  اضافه الى انها تحترم تعهداتها لحمايه المخيمات الفلسطينيه اثر الخروج لبنان وانتهى الامر  الى انسحاب اميركي مفاجيء للمجزره الصهيونيه الكتائبيه البشعه صبرا وشاتيلا</t>
+  </si>
+  <si>
+    <t>ودان المسؤول السياسيل الجماعه الاسلاميه الجنوبالشيخ صلاح الدين ارقه دان  المجزرهمعتبرا انها تضاف الي سلسلهالمجازر ارتكبها العدو الاسرائيليدير ياسين وصبرا  وشاتيلا
+  ودان المسؤول السياسي الجماعه الاسلاميه الجنوب الشيخ صلاح الدين ارقه دان  المجزره معتبرا انها تضاف الى سلسله المجازر ارتكبها العدو الاسرائيلي دير ياسين وصبرا  وشاتيلا</t>
+  </si>
+  <si>
+    <t>بيروت تعرضتللمجازر بدايه الفتنه لبنانالسبت الاسود وحتي صبرا وشاتيلاوالضاحيه تعاني  اليوم مجزره جديدهمخيفه جداء لان الخصومه المرهضمن اهل بيروت وهذه  الفتنه تخدمقطما الا العدو الاسرائيلي
+  بيروت تعرضت للمجازر بدايه الفتنه لبنان السبت الاسود وحتى صبرا وشاتيلا والضاحيه تعاني  اليوم مجزره جديده مخيفه جدا لان الخصومه المره ضمن اهل بيروت وهذه  الفتنه تخدم قطعا الا العدو الاسرائيلي</t>
+  </si>
+  <si>
+    <t>ان حقيقه حصل مجازرفعليه دفعنا شهيد وجريحا فضلا تججير معظم  ابناءاننا نؤكد العيش المشتركونحن كفلسطينيين لدينافرد ايه مجزره ابتداءدير ياسين  وانتهاء بمجازر صبراوشاتيلاء ولم تكن يوم الايام ايهقريه مسيحيه مهدده  الفلسطينيينبحكم انتمائها المذهبي واهالي دربالسيم والميه وميه ومغدوشهجيداء وان النار  كانت تاتيمغدوشه وتلالها كانت تحرق المخيموتحملنا الخسائر والاستنزاف حفاظااالعيش المشترك
+  ان حقيقه حصل مجازر فعليه دفعنا شهيد وجريحا فضلا تهجير معظم  ابنائنا اننا نؤكد العيش المشترك ونحن كفلسطينيين لدينا فرد ايه مجزره ابتداء دير ياسين  وانتهاء بمجازر صبرا وشاتيلا ولم تكن يوم الايام ايه قريه مسيحيه مهدده  الفلسطينيين بحكم انتمائها المذهبي واهالي درب السيم والميه وميه ومغدوشه جيدا وان النار  كانت تاتي مغدوشه وتلالها كانت تحرق المخيم وتحملنا الخسائر والاستنزاف حفاظا العيش المشترك</t>
+  </si>
+  <si>
+    <t>وتحدث الشيخ عبد الحليم زيدانخطبه القاما جامع البوابه التحتاصيدا تغيير  الواجهاتالسياسيه والعسكريه للقشواتاللبنانيه وقال تغهير الوجوهانكشفت واقتضحدت باخري جديدهنسبيا يمكنه  ان يفش شعبنا ذاقمراره الحقد تكنه القواتاللبنانيه وهذا التعويم ولد  فاشلالانهم يجدوا وجها بينهم انظفواطهر قائد مجزره صبرا وشاتيلاوانتقد المارونيه  السياسيهواعتبر ان حزب الكتائب القواتاللبنانيه مدرسه واحده تغيرتالقياده والواجهه وانهما  عملهواحده
+  وتحدث الشيخ عبد الحليم زيدان خطبه القاها جامع البوابه التحتا صيدا تغيير  الواجهات السياسيه والعسكريه للقوات اللبنانيه وقال تغيير الوجوه انكشفت واتضحدت باخرى جديده نسبيا يمكنه  ان يغش شعبنا ذاق مراره الحقد تكنه القوات اللبنانيه وهذا التعويم ولد  فاشل الا انهم يجدوا وجها بينهم انظف واطهر قائد مجزره صبرا وشاتيلا وانتقد المارونيه  السياسيه واعتبر ان حزب الكتائب القوات اللبنانيه مدرسه واحده تغيرت القياده والواجهه وانهما  عمله واحده</t>
+  </si>
+  <si>
+    <t>اننا نشكالشك التقاف الجمهور المسيحيحول الرمز الجديد وتكريسه للصفهالتمثيليه يدعيها  لنفسه نظراالي صيته الحميد واقتران اسمهبمجزره صبرا وشاتيلا ضجالعالم وكشفت  دوره وساكلالاعلام العالميه تظن ان المجتمعالمسيحي الغني بالرجال اصبح عاقرالهذا  الحد
+  اننا نشك الشك التفاف الجمهور المسيحي حول الرمز الجديد وتكريسه للصفه التمثيليه يدعيها  لنفسه نظرا الى صيته الحميد واقتران اسمه بمجزره صبرا وشاتيلا ضج العالم وكشفت  دوره وسائل الاعلام العالميه تظن ان المجتمع المسيحي الغني بالرجال اصبح عاقرا لهذا  الحد</t>
+  </si>
+  <si>
+    <t>وعن نظرته الي التغيرات الاخيرهالقوات اللبنانيه قال ان ايعادجعجع الواجهه  ومجيء ايلي حبيقهالا تبديل للاقنعه لامتصاصالنقمه المجتمع المسيحي المحليوالغربي وحبيقه  منفذ مجزره المعصرصبرا وشاتيلا ويداه ملطختانبدماء المواطنين وشخصيته معروفهيانها احدي  الادوات الاسرائيليهالقوات اللبنانيه
+  وعن نظرته الى التغيرات الاخيره القوات اللبنانيه قال ان ايعاد جعجع الواجهه  ومجيء ايلي حبيقه الا تبديل للاقنعه لامتصاص النقمه المجتمع المسيحي المحلي والغربي وحبيقه  منفذ مجزره العصر صبرا وشاتيلا ويداه ملطختان بدماء المواطنين وشخصيته معروفه يانها احدي  الادوات الاسرائيليه القوات اللبنانيه</t>
+  </si>
+  <si>
+    <t>وذكرتحصل المناطق الشرقيه ضداللبنانيين والفلسطينيين ومجزرهصبرا وشاتيلاء وبمساعده حزبالكتائب وقواته  القوات الاسرائيليهاثناء اجتياحها للبنان
+  وذكرت حصل المناطق الشرقيه ضد اللبنانيين والفلسطينيين ومجزره صبرا وشاتيلا وبمساعده حزب الكتائب وقواته  القوات الاسرائيليه اثناء اجتياحها للبنان</t>
+  </si>
+  <si>
+    <t>وكان البطريرك حكيم صرح اتنانهنيء السيد حبيقه جراتهويقظته الجديده سوريا  وانكانت جاءت متاخره واعلن اننيساغتنم زيارتي لدمشق لمعرفه نياتالمسؤولين السوريين  التبدلالجذري المفاجيء اعلنه السيدوهنا ذكر العميد اذه البطريركحكيم ببعض ورد  تقرير كاهانمجزره مخيمي صبرا وشاتيلاءوبالتحقيق المجزره نشرهاهنون كابليوك الموندوبالمقابل نشرته  مجله تايمتشرين الاول المجزره ءومقال بيار لوك سيقيون مجلهتموانياج كريتيان  تاريخكانون الاول تحت عنوان “شارونكان يعرفء وكذلك الجميل
+  وكان البطريرك حكيم صرح اننا نهنئ السيد حبيقه جرأته ويقظته الجديده سوريا  وان كانت جاءت متاخره واعلن انني ساغتنم زيارتي لدمشق لمعرفه نيات المسؤولين السوريين  التبدل الجذري المفاجئ اعلنه السيد وهنا ذكر العميد ان البطريرك حكيم ببعض ورد  تقرير كاهان مجزره مخيمي صبرا وشاتيلا وبالتحقيق المجزره نشره اهنون كابليوك الموند وبالمقابل نشرته  مجله تايم تشرين الاول المجزره ومقال بيارلوك سيقيون مجله تموانياج كريتيان  تاريخ كانون الاول تحت عنوان شارون كان يعرف وكذلك الجميل</t>
+  </si>
+  <si>
+    <t>كفتنا مجزرهصبرا وشاتيلا ايدي الكتائبءوتجري اليوم مجزره جديده صبراوشاتيلاء فلحسابتصر  يجري بهروتمعركه طائفيه انها معركهاسرائيل ضد المسلمين جميعا وضدالوحده الاسلاميه
+  كفتنا مجزره صبرا وشاتيلا ايدي الكتائب وتجري اليوم مجزره جديده صبرا وشاتيلا فلحساب تصر  يجري بيروت معركه طائفيه انها معركه اسرائيل ضد المسلمين جميعا وضد الوحده الاسلاميه</t>
+  </si>
+  <si>
+    <t>عين بعالوجه اهالي عين بعال الي رئيسحركه امل الوزير نبيه  بري البياناذ نستنكر بشده الاعتداء الاثمحركه امل المجاهدهالمؤمنه نتوقف طويلا  امامالبندقيه الحاهده ظهرت حديثاءونتساءل اين كانت ايام مجزره صبراوشاتيلا لماذا  تطلق رصاصهواحده العدو الصهيونيلذلك فاننا نصر قطع اليدالعميله تلوثت بدماء  الابرياءوالاطفال والنساء معاهدين اللهورسوله السير خطي الامامالصدر المغيب واضعين امكاناتناالبشريه  والماديه تصرفكم سائلينالمولي عز وجل ينصركم ويسددخطاكم خير الامهتكالبت عليها  عناصر الشر وجيوشضالحاشقدين حدب وصوب
+  عين بعال وجه اهالي عين بعال الى رئيس حركه امل الوزير نبيه  بري البيان اذ نستنكر بشده الاعتداء حركه امل المجاهده المؤمنه نتوقف طويلا  امام البندقيه الحاهده ظهرت حديثا ونتساءل اين كانت ايام مجزره صبرا وشاتيلا لماذا  تطلق رصاصه واحده العدو الصهيوني لذلك فاننا نصر قطع اليد العميله تلوثت بدماء  الابرياء والاطفال والنساء معاهدين الله ورسوله السير خطى الامام الصدر المغيب واضعين امكاناتنا البشريه  والماديه تصرفكم سائلين المولي عز وجل ينصركم ويسدد خطاكم خير الامه تكالبت عليها  عناصر الشر وجيوش الحاقدين</t>
+  </si>
+  <si>
+    <t>فصبرا وشاتيلا رمزابشع مجزره التاريخ والعودهاليهما وتلطيخ ايدي حركه املمجددا  امر طباق وجناساللغه العربيهه مرفوض اعلامياخصوصا اذا كان الاعلام مجربا  وخبيرمثل اعلام عرفات
+  فصبرا وشاتيلا رمز ابشع مجزره التاريخ والعوده اليهما وتلطيخ ايدي حركه امل مجددا  امر طباق وجناس اللغه العربيه مرفوض اعلاميا خصوصا اذا كان الاعلام مجربا  وخبير مثل اعلام عرفات</t>
+  </si>
+  <si>
+    <t>اتسمت امس حرب المخيماتحركه امل والمقاتلينالفلسطينيين يومها التاسع ببعضالعنف فدارت  معارك عنيفه خصدضاجبهه مخيمي صبرا وشاتيلاتواتر معلومات مجزره ارتكبهامقاتلون فلسطهنيون  ضد مقاتلينامل وجنود اللواء السائسعمليه تسلل الي مستشفي دار العجزهالاسلاميه
+  اتسمت امس حرب المخيمات حركه امل والمقاتلين الفلسطينيين يومها التاسع ببعض العنف فدارت  معارك عنيفه ضد ضاجبه مخيمي صبرا وشاتيلا تواتر معلومات مجزره ارتكبها مقاتلون فلسطينيون  ضد مقاتلين امل وجنود اللواء السائس عمليه تسلل الى مستشفي دار العجزه الاسلاميه</t>
+  </si>
+  <si>
+    <t>لقد كان المئهسكان المخيم الشيعه وعندماحصلت مجزره القوات اللبنانيهصبرا وشاتيلا  سقط شيعيا بينهم
+  لقد كان المئه سكان المخيم الشيعه وعندما حصلت مجزره القوات اللبنانيه صبرا وشاتيلا  سقط شيعيا بينهم</t>
+  </si>
+  <si>
+    <t>تحدث المسؤول الاشتراكيالتطورات لبنان فقال ان لوفصعب جدا وان يجري  بهروتنسخه جديده صبرا وشاتيلا ويشكلماساه بالتسبه الي الالفلسطيني اشاره الي  تكرارمجزره المخيمين
+  تحدث المسؤول الاشتراكي التطورات لبنان فقال ان الوضع صعب جدا وان يجري  بيروت نسخه جديده صبرا وشاتيلا ويشكل ماساه الى الفلسطيني اشاره الى  تكرار مجزره المخيمين</t>
+  </si>
+  <si>
+    <t>مجزره صبرا وشاتيلا عامنفذها شارون بقوات مشتركه جيشهو القوات الليناج  مجزره صبرا وشاتيلا وبرجالبراجنه عام تنفذها ماديا وبشريازمر فاشيه حركه  امل والجيشاللبناني اللواء السادس انسجاماالمشروع السياسي الصهيوني
+  مجزره صبرا وشاتيلا عام نفذها شارون بقوات مشتركه جيش هو القوات الليناج  مجزره صبرا وشاتيلا وبرج البراجنه عام تنفذها ماديا وبشريا زمر فاشيه حركه  امل والجيش اللبناني اللواء السادس انسجاما المشروع السياسي الصهيوني</t>
+  </si>
+  <si>
+    <t>المؤتمر جاء بعدماانطلقت المراه الفلسطينيهمجزره صبرا وشاتيلا لتقولوامعتصماه فكان المرد  الدعوه اليالقمه
+  المؤتمر جاء بعدما انطلقت المراه الفلسطينيه مجزره صبرا وشاتيلا لتقول وامعتصماه فكان المرد  الدعوه الى القمه</t>
+  </si>
+  <si>
+    <t>لبنان صينيه فضه الياسرائيل وكان عرابا لمجازر صبراوشاتيلا والصقراء وكان  مساهها كبيراوراء الستار مجزره اهدنذهب ضحيتها ولدكم وزوجته وابئنتهالطفله وكان  سببا مجازر المتنوبعض قري جبيل
+  لبنان صينيه فضه الى اسرائيل وكان عرابا لمجازر صبرا وشاتيلا والصقراء وكان  مساهها كبيرا وراء الستار مجزره اهدن ذهب ضحيتها ولدكم وزوجته وابنته الطفله وكان  سببا مجازر المتن وبعض قرى جبيل</t>
+  </si>
+  <si>
+    <t>عندما يكون احد اطرافالتحالف الرمز الاسرائيلي رمز مجزرهصبرا وشاتيلا يمكن  انموقع الحوار موقفنا
+  عندما يكون احد اطراف التحالف الرمز الاسرائيلي رمز مجزره صبرا وشاتيلا يمكن  ان موقع الحوار موقفنا</t>
+  </si>
+  <si>
+    <t>ومنعت مرورالسيارات سوق الخضر باستثناءالسيارات تنقل الخضرووزعت قصاصات باسم جبعهالانقاذ  اللجنه الشعبيهيسقط اطفالنا ضحايا الرعوئهوالطيش ساهموا منع اطلاق التارالهواء” كان  صبرا وشاتيلارصاص وقعت المجزره القناعالليل والنهار وبعد زوال الاحتلالخدمه للجبناء  والعملاءاحمد مننشالحركه منطقه بنايات رستم شارععبد المنور حاره حريك وكانت  مزودهرشاهات ثقيله راحت تطلق النارالهواء وعلي منازل الفلسطينهينانطلقت مجموعات همجيه  لتقتحمبيوت العائلات الامنه وكما فعلالصهاينه المحتلون مضيءفعلوا هناك
+  ومنعت مرور السيارات سوق الخضر باستثناء السيارات تنقل الخضر ووزعت قصاصات باسم جبهه لانقاذ  اللجنه الشعبيه يسقط اطفالنا ضحايا الجيش ساهموا منع اطلاق النار الهواء كان  صبرا وشاتيلا رصاص وقعت المجزره القناع الليل والنهار وبعد زوال الاحتلال خدمه للجبناء  والعملاء احمد منش الحركه منطقه بنايات رستم شارع عبد المنور حاره حريك وكانت  مزوده رشاشات ثقيله راحت تطلق النار الهواء وعلى منازل الفلسطينيين انطلقت مجموعات همجيه  لتقتحم بيوت العائلات الامنه وكما فعل الصهاينه المحتلون مضى فعلوا هناك</t>
+  </si>
+  <si>
+    <t>لهذانحتاج الي التنسيق نستطيع انيحمي بعضنا بعضا ولكي نكون قالالله  الله يحب يقاتلونسبيله صفا لكانهم بنيان مرصوصيحبه الله كلكم تقولونانكم  تريدون قتال اسرائيل ونحنتصدظكم لذا وفروا القتالوقال علينا ان نفهم  ان قامبمجزره صبرا وشاتيلا وخطط لمجزرهيئر العبد ومجازر الضاحيه وبيروتيمكن  ان يخلصوا للانسان الخرءالاوضاع لمسك الاوراقستضيع الاوراق
+  لهذا نحتاج الى التنسيق نستطيع ان يحمي بعضنا بعضا ولكي نكون قال الله  يحب يقاتلون سبيله صفا لكنهم بنيان مرصوص يحبه الله كلكم تقولون انكم  تريدون قتال اسرائيل ونحن نصدكم لذا وفروا القتال وقال علينا ان نفهم  ان قام بمجزره صبرا وشاتيلا وخطط لمجزره بئر العبد ومجازر الضاحيه وبيروت يمكن  ان يخلصوا للانسان الحر الاوضاع لمسك الاوراق ستضيع الاوراق</t>
+  </si>
+  <si>
+    <t>اضراب غدا يف عينالحلوهمسيره نظمنها الشبيبه الفلسطينيهذكري مجزره صبرا وشائيلاصيدا  النهارنظمت امس منظمه الشبيبهالفلسطينيه مخيم عين الحلومعسكر الشهيد معروف سعد  ءمسيره طالبيه وكشفيه بدعوهجبمه الانقاذ الوطني الفلسطينيالنكري الثالثه لمجزره مخيميصبرا  وشاتيلاورقع المشاركون اعلامالبنانيه وفلسطينيه ولافتات تندداحمد متنشبمرتكبي المجزره ومنها دماء  شعبنااظهر اطهركم ايها الشارونيونو الثوره ستستمر رغم المجازرالنصر والتحرير
+  اضراب غدا في عين الحلوه مسيره نظمنها الشبيبه الفلسطينيه ذكرى مجزره صبرا وشاتيلا صيدا  النهار نظمت امس منظمه الشبيبه الفلسطينيه مخيم عين الحلوه معسكر الشهيد معروف سعد  مسيره طالبيه وكشفيه بدعوه جبهه الانقاذ الوطني الفلسطيني الذكرى الثالثه لمجزره مخيمي صبرا  وشاتيلا ورفع المشاركون اعلام لبنانيه وفلسطينيه ولافتات تندد احمد متنش بمرتكبي المجزره ومنها دماء  شعبنا اظهر اطهركم ايها الشارونيونون الثوره ستستمر رغم المجازر النصر والتحرير</t>
+  </si>
+  <si>
+    <t>جبهه الانقاذتدعو الي اضرابصيدا النهاردعت قياده الجنوب جبههالاتنقاذ الوطني الفلسطيني  الياضراب عام اليوم مخيم عين الحلوهمعسكر الشهيد معروف سعد ءاستنكارا  لمجزره صبرا وشاتيلاو المجازر ترتكب ضد مخيماتناووزعت الجبهه امس بيانا  قالتايلول يحملطياته معاني والاما وتضحيات جساماءمعاني الصمود والبطوله معاني قراررفض  خروج المقاتلين بيروتمعاني رفض خيار عرفات سياسهالمفاوضات
+  جبهه الانقاذ تدعو الى اضراب صيدا النهار دعت قياده الجنوب جبهه الانقاذ الوطني الفلسطيني  الى اضراب عام اليوم مخيم عين الحلوه معسكر الشهيد معروف سعد استنكارا  لمجزره صبرا وشاتيلا والمجازر ترتكب ضد مخيماتنا ووزعت الجبهه امس بيانا  قالت ايلول يحمل طياته معاني والامل وتضحيات معاني الصمود والبطوله معاني قرار رفض  خروج المقاتلين بيروت معاني رفض خيار عرفات سياسه المفاوضات</t>
+  </si>
+  <si>
+    <t>وقال البيان ان ثلاث ذكريات تمرعلينا الاسبوع الاولي ذكري راسالسنه  المجريه تضعنا اجواءبدايات الدعوه الاسلاميه والثانيهذكري عاهوراء تضعنا اجواءمحاربه الظلم  والظالم قلهالعدد والعده والذكري الثالثهمجزره صبرا وشاتيلا ارتكبهاالصجاينه وعملاؤهم اللوات  اللبنائيهباشراف ايلي حبيقه يريد تبديللونه اليوم ويقلول انه اصبح الخيارالعربي
+  وقال البيان ان ثلاث ذكريات تمر علينا الاسبوع الاولي ذكري راس السنه  الهجريه تضعنا اجواء بدايات الدعوه الاسلاميه والثانيه ذكرى عاشوراء تضعنا اجواء محاربه الظلم  والظالم قله العدد والعده والذكرى الثالثه مجزره صبرا وشاتيلا ارتكبها الصهاينه وعملاؤهم القوات  اللبنانيه باشراف ايلي حبيقه يريد تبديل لونه اليوم ويقول انه اصبح الخيار العربي</t>
+  </si>
+  <si>
+    <t>احتفال الجماعهعين الحلوهصيدا النهارمناسبه راس السنه الهجريهوذكري مجزره صبرا وشاتيلا  اقامتالجماعه الاسلاميه احتفالا خطابيامخيم عين الحلوه حضره لفيفالعلماء وجمهور
+  احتفال الجماعه عين الحلوه صيدا النهار مناسبه راس السنه الهجريه وذكرى مجزره صبرا وشاتيلا  اقامت الجماعه الاسلاميه احتفالا خطابيا مخيم عين الحلوه حضره لفيف العلماء وجمهور</t>
+  </si>
+  <si>
+    <t>وتحدث امين الجبهه الاسلاميهالشيخ محرم العارفي فوصف مجزرهصبرا وشاتيلا بانها  مؤامره ضدالاسلام والمسلمين لبنانوربما تصادما اخوانهم اللبناتيينوراي ان المشاريع والطروخاتاكثر  خطوه مشوار الالف ميل
+  وتحدث امين الجبهه الاسلاميه الشيخ محرم العارفي فوصف مجزره صبرا وشاتيلا بانها  مؤامره ضد الاسلام والمسلمين لبنان وربما تصادما اخوانهم اللبنانيين وراى ان المشاريع والطروحات اكثر  خطوه مشوار الالف ميل</t>
+  </si>
+  <si>
+    <t>نظمه التحرب وجبهات فلسطينيهدانت مجزره صبراوشائيلاوغيرهاالذكري الثالثه لمجزره مخيميصبرا وشاتيلاء  دانت منظمه التحريرالفلسطينيه وجبهات وتنظيماتالمجازر والمجازر ارتكبت حارهحريك والاعتداءات برج  البراجنهمنظمه التحريروجاء بيان منظمه التحريرتحل الذكري الثالثه لمجازر صبراوشاتيلا وشعبنا  يواصل نضائه الباسلالدؤوب اجل انتزاع حقوقه الوطنيهففي الوطن المحتل تنتفض  جماجهرتاضد الاحتلال الصجيوني حركهجماهيريه واسعه ينخرط شعبناباسره وتمارس طلائعه النضال  المسلحضد العدو الصهيوني الغاصب بكلالاشكال والاساليب المتاحه
+  نظمه الحزب وجبهات فلسطينيه دانت مجزره صبرا وشاتيلا وغيرهاالذكري الثالثه لمجزره مخيمي صبرا وشاتيلا  دانت منظمه التحرير الفلسطينيه وجبهات وتنظيمات المجازر والمجازر ارتكبت حاره حريك والاعتداءات برج  البراجنه منظمه التحرير وجاء بيان منظمه التحرير تحل الذكرى الثالثه لمجازر صبرا وشاتيلا وشعبنا  يواصل نضاله الباسل الدؤوب اجل انتزاع حقوقه الوطنيه في الوطن المحتل تنتفض  جماهيرنا ضد الاحتلال الصهيوني حركه جماهيريه واسعه ينخرط شعبنا باسره وتمارس طلائعه النضال  المسلح ضد العدو الصهيوني الغاصب بكل الاشكال والاساليب المتاحه</t>
+  </si>
+  <si>
+    <t>وذكر بيان الجبهه الشعبيهبمجازر ايلول الاردن اضاقه اليمجزره صبرا وشاتيلاء  معتبرا انهاافرزت دروسا غنيه اجل استمرارالنضال والكفاح
+  وذكر بيان الجبهه الشعبيه بمجازر ايلول الاردن اضافه الى مجزره صبرا وشاتيلا  معتبرا انها افرزت دروسا غنيه اجل استمرار النضال والكفاح</t>
+  </si>
+  <si>
+    <t>وذكر بمجزره صبراوشاتيلا محييا ارواح الابرياء
+  وذكر بمجزره صبرا وشاتيلا محييا ارواح الابرياء</t>
+  </si>
+  <si>
+    <t>قال قليلات الذكريالثالثه لاجتياح اقسواتالغزو الصهيوني بيروت الوطنيهوالاسلاميه وفي ذكري  مجزره مخيميصبرا وشاتيلاء تبدو اليوم ملامحمواجهه مصيريه ازاء مستقبلالبلد وازاء  تظرير مصيره ايضا ظلاستمرار الاحتلال الاسراكيلي لجزءالجنوب اللبناني وتعتبر ان  اي مدخللحل الازمه او اي مشروع سياسي يطرحيجب ينطلق مبدا  استكمالتحرير الارض القزاه
+  قال قليلات الذكرى الثالثه لاجتياح قوات الغزو الصهيوني بيروت الوطنيه والاسلاميه وفي ذكرى  مجزره مخيمي صبرا وشاتيلا تبدو اليوم ملامح مواجهه مصيريه ازاء مستقبل البلد وازاء  تحرير مصيره ايضا ظل استمرار الاحتلال الاسرائيلي لجزء الجنوب اللبناني وتعتبر ان  اي مدخل لحل الازمه او اي مشروع سياسي يطرح يجب ينطلق مبدا  استكمال تحرير الارض الغزاه</t>
+  </si>
+  <si>
+    <t>الجبهه الديموقراطيهجاعنا الجبهه الديموقراطيهلتحرير فلسطين ان البيان نسباليها ذكري مجزره  صبرا وشاتيلانهار الاربعاء الماضي انمال اللجنه الشعبيه لمخيم الجليل”
+  الجبهه الديموقراطيه لتحرير فلسطين ان البيان نسب اليها ذكرى مجزره  صبرا وشاتيلا نهار الاربعاء الماضي انما اللجنه الشعبيه لمخيم الجليل”</t>
+  </si>
+  <si>
+    <t>حل لاخ يلم لوندي الوكلا العهديبتالصوات تهجيرمساي جبيلفضل الله ارال  ستوسع اشرماولن بمد يد الي مركي الجازراعلن العلامه السيد محمد  حسينفضل الله انه يرفض ان يكونخطط لمجزره صبرا وشاتيلا ومجازر  تلالزعثر والتبعه والمسلخ ونفذهاالممثل تمتد اليهاليد واتهم القوات اللبنانيهبتهجير المسلمين  جبيل وحرمبيع اراضيهم محذرا انابرياء مناطق اشخري سيدقعونالثمن ونبه الي  ان اسرائيل تسعيالي توسيع الشريط الحدودي وبناءمستوطنات الجنوباستهل فضل الله  خطبه الجمعهالقاها مسجد الامام الرضابكر العبد
+  اعلن العلامه السيد محمد  اعلن العلامه السيد محمد  حسين فضل الله انه يرفض ان يكون خطط لمجزره صبرا وشاتيلا ومجازر  تلال زعتر والتبعه والمسلخ ونفذها الممثل تمتد اليه اليد واتهم القوات اللبنانيه بتهجير المسلمين  جبيل وحرم بيع اراضيهم محذرا ان ابرياء مناطق اخرى سيدفعون الثمن ونبه الى  ان اسرائيل تسعى الى توسيع الشريط الحدودي وبناء مستوطنات الجنوب استهل فضل الله  خطبه الجمعه القاها مسجد الامام الرضا بئر العبد</t>
+  </si>
+  <si>
+    <t>ايام مرت علينا ذكري مجزرهتشابه صورها واشكالجا مذبحهعاشوراء مجزره صبرا  وشاتيلامثل فيها باطفال فلسطينيينومسلمين لبنانيين حق وتبحتقيما نساء حوامل وشيوخ  وعجزهنون حق وذبح شباب عزلءالمجزره بلغت فظاعتهماووحشيتها ان اسرائيل افسحتالمجال  وربما خططتوكانت غطاء سياسيا وعسكريا لمنقام حاولت التبره واوجدتشكلا قانونيا  داخل اجهزتها يحاولالتحقيق ويحاكم قامتبريء نفسها امام العالم ضجهول المجزره
+  ايام مرت علينا ذكري مجزره تشابه صورها واشكالها مذبحه عاشوراء مجزره صبرا  وشاتيلا مثل فيها باطفال فلسطينيين ومسلمين لبنانيين حق وتبح تقيما نساء حوامل وشيوخ  وعجزه نون حق وذبح شباب عزل المجزره بلغت فظاعتهما ووحشيتها ان اسرائيل افسحت المجال  وربما خططت وكانت غطاء سياسيا وعسكريا لمن قام حاولت التبره واوجدت شكلا قانونيا  داخل اجهزتها يحاول التحقيق ويحاكم قام تبريئ نفسها امام العالم حول المجزره</t>
+  </si>
+  <si>
+    <t>وافادت وكاله رويتر ان اخرعرف ديفيسون انه كانكانون الاول متن  سفينهتولت اجلاء فدائيين موالين لرئيساللجنه التنفيذيه لمنظمه التحريرالفلسطينيه السيد ياسر  عرقاتالف وفيها انه انضم الي منظمهالتحرير رد فعل ثلاث ستواتامضاها  الولايات المتحده “يعبثحياك طيبه ضميراجتماعي وبعدما شاهد صورا لمجزرهصبرا وشاتيلا
+  وافادت وكاله رويتر ان اخر عرف ديفيسون انه كان كانون الاول متن  سفينه تولت اجلاء فدائيين موالين لرئيس اللجنه التنفيذيه لمنظمه التحرير الفلسطينيه السيد ياسر  عرفات الف وفيها انه انضم الي منظمه التحرير رد فعل ثلاث سنوات امضاها  الولايات المتحده “يعبث حياك طيبه ضمير اجتماعي وبعدما شاهد صورا لمجزره صبرا وشاتيلا</t>
+  </si>
+  <si>
+    <t>وطرح ثلاثه اسئلهتزال صور المجازر المتكررهحق شعبنا ومجزره صبرا وشاتيلا  تزالماثله امامنا يضمن سلامهالمخيمات وسواحل المخيماتلبتان بعدما راينا الساحل التونسيهمدقا  للطيران الصهيوني رغم انساكني حمام الشط نفوا انفسهمسبيل القضيهلبنان ام  انه ارفك وله حقوقمواطني الارض اللبنانيه وهل ياخذدوره لبنان سورياوراي  ان الاجابه تكونانذاك خيانات الدول العربيهوالتي احتنت جزءا ثمييا لبنانالجنوب
+  وطرح ثلاثه اسئله تزال صور المجازر المتكرره حق شعبنا ومجزره صبرا وشاتيلا  تزال ماثله امامنا يضمن سلامه المخيمات وسواحل المخيمات لبنان بعدما راينا الساحل التونسيه مدقا  للطيران الصهيوني رغم ان ساكني حمام الشط نفوا انفسهم سبيل القضيه لبنان ام  انه ارفك وله حقوق مواطني الارض اللبنانيه وهل ياخذ دوره لبنان سوريا وراي  ان الاجابه تكون انذاك خيانات الدول العربيه والتي احتنت جزءا ثمينا لبنان الجنوب</t>
+  </si>
+  <si>
+    <t>واذا قررنا انتموت فلن تستطيع اميركا ان تفعلولاحظ المراقبون ان  كلام الزعيمالليبي يتناقض نقيه تورط ليبياهجومي روما وقيينا ورفضهالاتهامات بانه  قدم تسهيلات لتدريبجماعه ابو نضال المنشقه دركهوكان القذاقي صرح مقابلهاجراها  معه التلفزيون الالماني الغربياول امس انه يفرقالهجومين مطاري روما وفييناو  حمامات الدم مكان اخرالعالم اشاره الي جنوب اقروالفزو الاميركي لجزيره  غرينادا ومجزرهمخيمي صبرا وشاتيلا عامليم المهرجان مناسبه ذكريرئيس المصري الراحل  جمالعبد الناصر
+  واذا قررنا ان تموت فلن تستطيع اميركا ان تفعل ولاحظ المراقبون ان  كلام الزعيم الليبي يتناقض نقيه تورط ليبيا هجومي روما وفيينا ورفضها لاتهامات بانه  قدم تسهيلات لتدريب جماعه ابو نضال المنشقه دركه وكان القذاقي صرح مقابله اجراها  معه التلفزيون الالماني الغربي اول امس انه يفرق الهجومين مطاري روما وفييناو  حمامات الدم مكان اخر العالم اشاره الى جنوب اقر والغزو الاميركي لجزيره  غرينادا ومجزره مخيمي صبرا وشاتيلا المهرجان مناسبه ذكر يرئيس المصري الراحل  جمال عبد الناصر</t>
+  </si>
+  <si>
+    <t>وذكربمجزره مخيمي صبرا وشاتيلا قتلشخص شيوخا ونساءواطفالا الفلسطينيين شخصاعائله مقداد  اللبنانيه
+  وذكر بمجزره مخيمي صبرا وشاتيلا قتل شخص شيوخا ونساء واطفالا الفلسطينيين شخصا عائله مقداد  اللبنانيه</t>
+  </si>
+  <si>
+    <t>واشار الي ان شارون مسؤولمجزره مخيمي صبرا وشاتيلا عاموالي بيغن  مسؤول مذبحه ديرباسين قطاع غزه عامولم يستبعد ان تشن اسرائيلهجوما  ليبيا لان هدف اسرائيلافساد استقرار البخر الاييضالمتوسط وامنه
+  واشار الى ان شارون مسؤول مجزره مخيمي صبرا وشاتيلا عام والى بيغن  مسؤول مذبحه دير باسين قطاع غزه عام ولم يستبعد ان تشن اسرائيل هجوما  ليبيا لان هدف اسرائيل افساد استقرار البحر الاييض المتوسط وامنه</t>
+  </si>
+  <si>
+    <t>ورات ان يؤكد ان القويارتكبت مجزره صبرا وشاتيلاءوقبلها استباحت مخيم  تل الزعتروالنبعه وبرج حمود تريد عطي ملفاجرامها بعديا امتهنت سفك  دماءتعقد لجنه امالي المخطوفينظهر غد الاثنين مؤتمرا صحافيا دارنقابه الصحافه  ترد اعلانالقوات اللبنانيه انه يعد لديهاوقال مصدر مسؤول حزب اللهتصريح  ادلي المستضعفونوحدهم يتابعون قضيهابنائهم المخطوشينء وهم ومدهمالمعنيون اساسا بكشف مصيرهموتحديد  المجرم الحقيقي المسؤولالجريمه البشعه
+  ورات ان يؤكد ان القوى ارتكبت مجزره صبرا وشاتيلا وقبلها استباحت مخيم  تل الزعتر والنبعه وبرج حمود تريد عطي ملف اجرامها بعدما امتهنت سفك  دماء تعقد لجنه اهالي المخطوفين ظهر غد الاثنين مؤتمرا صحافيا دار نقابه الصحافه  ترد اعلان القوات اللبنانيه انه يعد لديها وقال مصدر مسؤول حزب الله تصريح  ادلى المستضعف ونوحدهم يتابعون قضيه ابنائهم المخطوفين وهم ومدهم المعنيون اساسا بكشف مصيرهم وتحديد  المجرم الحقيقي المسؤول الجريمه البشعه</t>
+  </si>
+  <si>
+    <t>لقد بلغالاعتداء الاستعماري الصعليبيوالههودي نروته احتلال لبنانوعاصمته عام اذ دخل  الجيشالصهيوني بيروت مرتكيا عملاكهالصغار الصليبيين صبرا وشاتيلاوكل مكان داسته دباباتهم  وارجلهممجزره بشعه
+  لقد بلغ الاعتداء الاستعماري الصليبي واليهودي ذروته احتلال لبنان وعاصمته عام اذ دخل  الجيش الصهيوني بيروت مرتكبا عملائه الصغار الصليبيين صبرا وشاتيلا وكل مكان داسته دباباتهم  وارجلهم مجزره بشعه</t>
+  </si>
+  <si>
+    <t>وهذا يعني المؤلف انتصارمنظمه التحرير الفلسطينيه اذ خسرتمواقعها الجنوب اجليت  قواتهابيروت توفر غطاء امنياللمدتيين الفلسطينيين بقوالبنانء فكانت مجزره صبرا وشاتيلاهبوطا  فاعليه المنظمه وانحساراامكاناتهما
+  وهذا يعني المؤلف انتصار منظمه التحرير الفلسطينيه اذ خسرت مواقعها الجنوب اجليت  قواتها بيروت توفر غطاء امنيا للمدنيين الفلسطينيين بقوا لبنان فكانت مجزره صبرا وشاتيلا هبوطا  فاعليه المنظمه وانحسار امكاناتهما</t>
+  </si>
+  <si>
+    <t>واصابالدول الكبري الصدع الشامل حتيالسياسه الاميركيه هيبتهاوصدقيتهاء هين تلجم اسرائيلاثناء  الاجتياحء ولم يقن ضمانهاوقوع مجزره صبرا وشاتيلا
+  واصاب الدول الكبرى الصدع الشامل حتى السياسه الاميركيه هيبتها وصدقيتها حين تلجم اسرائيل اثناء  الاجتياح ولم يكن ضمانها وقوع مجزره صبرا وشاتيلا</t>
+  </si>
+  <si>
+    <t>واكدت ان المقاتلين مخيمشاتيلا احبطوا عمليه تسلل الي شارعابو صالح  النمساويه وان قتيلا وجرحي بينهم اطفال سقطواودعت الجبهجه الشويوالشخصيات الوطنيه  والاسلاميه اليالتدخل الفعال لوضع حد للمجزرهالدائره ضد مخيمات شعبنااللجان الشعبيهووجمت  اللجان الشعبيهمخيمات برج البراجنه وصبرا وشاتيلانداء الي تائب رئيس المجلسالاسلامي  الشيعي الاعلي الشيخ محمدمهدي شمس الدين والعلامه السيدمحمد حسين فضل  الله تمنتعليهما ارسال لجنه لتقصي الحقائقيكون حكمهما عهدناه منصفاوعادلا اجل  وقف النزف
+  واكدت ان المقاتلين مخيم شاتيلا احبطوا عمليه تسلل الى شارع ابو صالح  النمساويه وان قتيلا وجرحى بينهم اطفال سقطوا ودعت الجبهه القوى والشخصيات الوطنيه  والاسلاميه الى التدخل الفعال لوضع حد للمجزره الدائره ضد مخيمات شعبنا اللجان الشعبيه ووجهت  اللجان الشعبيه مخيمات برج البراجنه وصبرا وشاتيلا نداء الى نائب رئيس المجلس الاسلامي  الشيعي الاعلي الشيخ محمد مهدي شمس الدين والعلامه السيد محمد حسين فضل  الله تمنت عليهما ارسال لجنه لتقصي الحقائق يكون حكمهما عهدناه منصفا وعادلا اجل  وقف النزف</t>
+  </si>
+  <si>
+    <t>ان المجزره الثالثهتحدث لمخيمات صبرا وشاتيلا وبرجالبراجنه
+  ان المجزره الثالثه تحدث لمخيمات صبرا وشاتيلا وبرج البراجنه</t>
+  </si>
+  <si>
+    <t>واعتبر تصويت مجلس الموزراءانتصارا شخصيا لشامير كانيمكن ان يؤدي تحظيق  تجربه الجئهرسميه الي مثل ادي اليه الت التحقيقمجزره مخيمي صبرا  وشاتيلاالعا ارييل شارون وزاره الدفاع
+  واعتبر تصويت مجلس الوزراء انتصارا شخصيا لشامير كان يمكن ان يؤدي تحقيق  تجربه الجئه رسميه الى مثل ادي اليه التحقيق مجزره مخيمي صبرا  وشاتيلا ارييل شارون وزاره الدفاع</t>
+  </si>
+  <si>
+    <t>وسافر كرم الي بوغوتا زيارلكولومبيا تستفرق اربعه ايام بناءدعوه رئيس  اتحاد صحافيي اميركااللاتيئيهاللقاء الوحدوي“ ممو معركه بيروتالذكري الرابعه للغزوالاسرائيلي لبيروت  والذكري الرابعهلمجزره صبرا وشاتيلاء والذكري الرابعهلانطلاقه المقاومه الوطنيه دعااللقاء الوحدوي  الي ندوه فكريهسياسيه الرابعه ظهر الاربعاءالمقبل التادي الثقافي العربيشارع عبد  العزيز بنايه ياردء تحتعنوان معركه بيروت التجربهيشترك الندوه الساده بشارهمرهج  الدكتور علي حسنء محمدكشلي ويديرها الدكتور معن زياده
+  وسافر كرم الى بوغوتا زياره لكولومبيا تستغرق اربعه ايام بناء دعوه رئيس  اتحاد صحافيي اميركا اللاتينيه اللقاء الوحدوي معركه بيروت الذكرى الرابعه للغزو الاسرائيلي لبيروت  والذكرى الرابعه لمجزره صبرا وشاتيلا والذكرى الرابعه لانطلاقه المقاومه الوطنيه دعا اللقاء الوحدوي  الى ندوه فكريه سياسيه الرابعه ظهر الاربعاء المقبل النادي الثقافي العربي شارع عبد  العزيز بنايه يارد تحت عنوان معركه بيروت التجرربه يشترك الندوه الساده بشار همرهج  الدكتور علي حسن محمد كشلي ويديرها الدكتور معن زياده</t>
+  </si>
+  <si>
+    <t>امام نصب شهداء مشيم برج لبراجنهالذكري الرابعه لمجزره مخيميصبرا وشاتيلاء  واستنكارا للقاءالاسكندريه الرئيس حسني مباركورئيس وزراء اسرائيل شمعون بيريزشهد مخيما  شاتيلا وبرج البراجنهمسيرات ووضع اكاليل نصبالشهداء
+  امام نصب شهداء مخيم برج البراجنه الذكرى الرابعه لمجزره مخيمي صبرا وشاتيلا  واستنكارا للقاء الاسكندريه الرئيس حسني مبارك ورئيس وزراء اسرائيل شمعون بيريز شهد مخيما  شاتيلا وبرج البراجنه مسيرات ووضع اكاليل نصب الشهداء</t>
+  </si>
+  <si>
+    <t>والقي “ابو عدنان كلمه باسمجبجه الانقاذ الوطني الفلسطينيتحدث معاني الذكريوالقي  راجي” كليه اعتبر انمجزره صبرا وشاتيلا شاهد حيهمجيه الارهاب الاميركي  الصهيونيوقال نرهد نذكر بمسلسلالعدوان الاميركي ضد الشصوبفالارهاب الامهركي الصهيوني جزءالسياسه  الرسميه لهذه الدول
+  والقى ابو عدنان كلمه باسم جبهه الانقاذ الوطني الفلسطيني تحدث معاني الذكرى والقي  راجي كلمه اعتبر ان مجزره صبرا وشاتيلا شاهد حيه مجيه الارهاب الاميركي  الصهيوني وقال نرهد نذكر بمسلسل العدوان الاميركي ضد التخوبف الارهاب الاميركي الصهيوني جزء السياسه  الرسميه لهذه الدول</t>
+  </si>
+  <si>
+    <t>الذكري الرابعه لغزو اسرائيلللبنان وذكري مجزره مخيمي صبراوشاتيلاء اقام انلقاء  الوحدوي ندوهالنادي الثقافي العربي عنوائهامفركه بيروت التجربهوالدلالات حضرها شخصيات وممثلوفاعليات  وجمع المهتمين
+  الذكرى الرابعه لغزو اسرائيل للبنان وذكرى مجزره مخيمي صبرا وشاتيلا اقام ان لقاء  الوحدوي ندوه النادي الثقافي العربي عنوانها معركه بيروت التجربه والدلالات حضرها شخصيات وممثلو فاعليات  وجمع المهتمين</t>
+  </si>
+  <si>
+    <t>تقد علمتنا بيروت الانخاف وانه يمكن الانتصار غلمتناتيع العلماءذكري مجزره  صبرا وشاتيلاءا لحم العلماء المسلمين بياناندوه اللماء الوحدوي وبياناتتوقيق العبداللهقال  ان يثير الالم النفوسان نكري هثه المجازر تترافق وحوارطرشان يجريه  اطراف يسمي الصفالوطني
+  لقد علمتنا بيروت الا نخاف وانه يمكن الانتصار علمتنا تبع العلماء ذكرى مجزره  صبرا وشاتيلا لحم العلماء المسلمين بيانا ندوه اللماء الوحدوي وبيانا تتوقيق العبد الله قال  ان يثير الالم النفوس ان نكري هذه المجازر تترافق وحوار طرشان يجريه  اطراف يسمي الصف الوطني</t>
+  </si>
+  <si>
+    <t>الذكري الرا بعه لمجزرده صيرا وشاتلامنظمات ورابطات المعركه البهودم لتضيه  الركزيه لل متناالذكري الرابعه لمجزره مخهميصبرا وشاتيلاء وزعت الجماعهالاسلاميه لبنان  امس بيانا دعتالي اخذ العبر والعظاتالمناسبه والنظر خلالها الي معالمالمستقبل
+  الذكرى الرابعه لمجزره صبرا وشاتيلا منظمات ورابطات المعركه البهود لتضيه  الركزيه لل متنا الذكري الرابعه لمجزره مخيمي صبرا وشاتيلا وزعت الجماعه الاسلاميه لبنان  امس بيانا دعت الى اخذ العبر والعظات المناسبه والنظر خلالها الى معالم المستقبل</t>
+  </si>
+  <si>
+    <t>وشدد البيان ان المجزرهستبقي وصمه عار جبين عربيوكل مسلم الي  ان يبعث الله يطهرالارض رجس اسرائيل ويعيد اليالامه عزتها وكرامتهاء  وتبقيالمعركه اليجود القضيهالمركزيه لامتنا المسلمه قدرمواجهه اشد الناس عداوه للنين  امتواغلها وحدها يجب تتوجه البنادقواضاف البيان حلفاء اسرائيلالقوات اللبنائيه كانوا  اداالجريمه صبرا وشاتيلا يزالونمكرهم وخداعهم يتلوئون حسبمناسبه ويبدلون اقنعتهم حسبظرف
+  وشدد البيان ان المجزره ستبقى وصمه عار جبين عربي وكل مسلم الى  ان يبعث الله يطهر الارض رجس اسرائيل ويعيد الى الامه عزتها وكرامتها  وتبقى المعركه اليهود القضيه المركزيه لامتنا المسلمه قدر مواجهه اشد الناس عداوه لللبنانيين  وحدها يجب تتوجه البنادق واضاف البيان حلفاء اسرائيل القوات اللبنانيه كانوا  اذا الجريمه صبرا وشاتيلا يزالون مكرهم وخداعهم يتلونون حسب مناسبه ويبدلون اقنعتهم حسب ظرف</t>
+  </si>
+  <si>
+    <t>وذكر بمجزره مخيمي صبرا وشاتيلاكانت خطه اسرائيليهكتائبيه وقال علينا ان  نتذكرتبحوا الاطفال والشيوخوالنساءء الفلسطينيين واللبنالهينتبح النفاج لتعرف معني السلامالاسرائيلي معني  السلام الكتاثبييدبر للمسلمين ونفهمالنوع التنسيقيتحركون دائره الحوار وجيش تمدتنسيقا سياسها  عسكريا امنيايدعوا المسلمين يحصلونبوصفها الخيار الوحيد للتدرهر شيفحسب لتوحيد القويوالجهات  الاهداف الواحدهاجل ان تحقق ارضيه حقيقيه تحوارفاعل
+  وذكر بمجزره مخيمي صبرا وشاتيلا كانت خطه اسرائيليه كتائبيه وقال علينا ان  نتذكر ذبحوا الاطفال والشيوخ والنساء الفلسطينيين واللبنانيين نتبحه الكفاح لتعرف معنى السلام الاسرائيلي معنى  السلام الكتائبي يدبر للمسلمين ونفهم النوع التنسيقي تحركون دائره الحوار وجيش تم تنسيقا سياسيا  عسكريا امنيا يدعوا المسلمين يحصلون بوصفها الخيار الوحيد للتدرهر شيف حسب لتوحيد القوى والجهات  الاهداف الواحده اجل ان تحقق ارضيه حقيقيه تحاور فاعل</t>
+  </si>
+  <si>
+    <t>التنظيم الناصريوللمناسبه وفي ذكري مجزرهمخيمي صبرا وشاتيلاء انلي المسؤولالسياسي الاتحاد  الاشتراكي العربيالتنظيم الناصري السيد منهرالصياد بتصريح اشاد المقاتلالوطني اللبناني والمقاتل  الفلسطينيوالمقاتل العربي السوري وقال انالجميع كانوا يعيشون لحظات النصررغم اجواء  الحصار المضروبوالتخائل العربي المفضوح تفاضيمؤامره خروج المقاومه ودخول انقوالمتعدده الجنسيه  افضت اليالدخول الاسرائيلي ومجازر صبراوشاتيلا
+  التنظيم الناصري وللمناسبه وفي ذكرلى مجزره مخيمي صبرا وشاتيلا انلي المسؤول السياسي الاتحاد  الاشتراكي العربي التنظيم الناصري السيد منهر الصياد بتصريح اشاد المقاتل الوطني اللبناني والمقاتل  الفلسطيني والمقاتل العربي السوري وقال ان الجميع كانوا يعيشون لحظات النصر رغم اجواء  الحصار المضروب والتخاذل العربي المفضوح تفاضي مؤامره خروج المقاومه ودخول القوى المتعدده الجنسيه  افضت الى الدخول الاسرائيلي ومجازر صبرا وشاتيلا</t>
+  </si>
+  <si>
+    <t>واشاد الدور يضطلعالاتحاد السوفياتي واليمنالديموقراطيه والجزائر اتجاه زائهالعقبات طريق وحده  المنظمهو الجهود الكبيره تبئل معنالتامين افضل الظروف لانعقاد دورهجديده للمجلس  ائوطني لتتويج وحدتناالوطنيه واعاده العلاقه منظمهالتنظيم الشعبي الناصري الدكتورنبيل الراعيء  فدعا الي استخلاصالدروس مجزره صبرا وشاتيلا لمنعتكرار المجازرء وتحصين الوضع  الوطنيوحمايته
+  واشاد الدور يضطلع الاتحاد السوفياتي واليمن الديموقراطيه والجزائر اتجاه ازاله العقبات طريق وحده  المنظمه والجهود الكبيره تبذل معنا لتامين افضل الظروف لانعقاد دوره جديده للمجلس  الوطني لتتويج وحدتنا الوطنيه واعاده العلاقه منظمه التنظيم الشعبي الناصري الدكتور نبيل الراعي  فدعا الى استخلاص الدروس مجزره صبرا وشاتيلا لمنع تكرار المجازر وتحصين الوضع  الوطني وحمايته</t>
+  </si>
+  <si>
+    <t>ونسالالسيد ياسر عرفات لماذا يستقبلكراس النظام وحزبه الامس بمثليستقبلك اليوم  حراره ولماذايريدك اليوم سجينا لبنانحق الخروج رقضك عندماكنت قضيه وثوره  شريفه اجلالقضيه الشريفه ام تراك نسيتمجزره عين الرمانه ومجازر صبراوشاتيلا
+  ونسال السيد ياسر عرفات لماذا يستقبل كراس النظام وحزبه الامس بمثل يستقبلك اليوم  حراره ولماذا يريدك اليوم سجينا لبنا نحق الخروج رفضك عندما كنت قضيه وثوره  شريفه اجل القضيه الشريفه ام تراك نسيت مجزره عين الرمانه ومجازر صبرا وشاتيلا</t>
+  </si>
+  <si>
+    <t>تمرعبر وجود استراتيجيه لبنائيه وعربيهواسلاميه محذرا خطر التمددالفلسطيني الي الجبل  والشوف واليطريق بيروت والمبقاع مستغرباالهجمه الاعلاميه والسياسيهوالعسكريه المنسقه كتائب مجزرهصبرا  وشاتيلا وعرفات
+  تمر عبر وجود استراتيجيه لبنانيه وعربيه واسلاميه محذرا خطر التمدد الفلسطيني الى الجبل  والشوف والى طريق بيروت والبقاع مستغربا الهجمه الاعلاميه والسياسيه والعسكريه المنسقه كتائب مجزره صبرا  وشاتيلا وعرفات</t>
+  </si>
+  <si>
+    <t>ونتساءل اصبح فتياسرائيل المدلل القوات اوبطل مجزره صبرا وشاتيلا ايلي  حبيظهصديقا حميما للنظام السورينسمح للسماسره الغرب بانيبيعوا الثوره الفلسطينيه ويسقطوا'بندقيتها
+  ونتساءل اصبح فتى اسرائيل المدلل القوات او بطل مجزره صبرا وشاتيلا ايلي  حبيقه صديقا حميما للنظام السوري نسمح للسماسره الغرب بان يبيعوا الثوره الفلسطينيه ويسقطوا بندقيتها</t>
+  </si>
+  <si>
+    <t>الانتكاسه طريقالاوزاعي حدثت قضاء وقدرا مؤامرهمكمن اهل الاوزاعي اناس طييونولم  يبدا ال المقداد بالمعركه وتكفيهممجزره شاتيلا وصبرا
+  الانتكاسه طريق الاوزاعي حدثت قضاء وقدرا مؤامره مكمن اهل الاوزاعي اناس طييون ولم  يبدأ آل المقداد بالمعركه وتكفيه مجزره شاتيلا وصبرا</t>
+  </si>
+  <si>
+    <t>كان مسؤولا بالمعننتتمه المنشور الصفحهوبين الرئيس السوري والسيد ايليحبيقه القائد  اللمسابق القواتاللبنانيه وتساءل اذا صار لقاءحسين مشروعا فلماذا نلتقيعرقات واذا  صار لقاء حبيقهابطال مجزره صبرا وشاتيلاء مشروعاخلماذا نلتقي شارون اذ  فارقحبيقه وشارون وزير الدفاعالاسرائيلي السابق
+  كان مسؤولا بالمعنن تتمه المنشور الصفحه وبين الرئيس السوري والسيد ايلي حبيقه القائد  اللم سابق القوات اللبنانيه وتساءل اذا صار لقاء حسين مشروعا فلماذا نلتقي عرفات واذا  صار لقاء حبيقه ابطال مجزره صبرا وشاتيلا مشروعا فلماذا نلتقي شارون اذ  فارق حبيقه وشارون وزير الدفاع الاسرائيلي السابق</t>
+  </si>
+  <si>
+    <t>وزعت بيانات ادائهباسم اللجنه الشعبيه مخيميصبرا وشاتيلا اللجنه الشعبيهالرشيديه اللجان  الشعبيه ”واصديرت سفاره الجمهوريهالاسلاميه بيروت بيانا اعتبرت“ان المجزره الوحشيه الجديدهارتكبتها  ظائرات العدو الاسرائيليعين الحلوه انما تعبر مدي الحقدوالهمجيه يتصفالعدو التاريخي  لامتنا
+  وزعت بيانات ادائه باسم اللجنه الشعبيه مخيمي صبرا وشاتيلا اللجنه الشعبيه الرشيديه اللجان  الشعبيه واصدرت سفاره الجمهوريه الاسلاميه بيروت بيانا اعتبرت ان المجزره الوحشيه الجديده ارتكبتها  طائرات العدو الاسرائيلي عين الحلوه انما تعبر مدى الحقد والهمجيه يتصف العدو التاريخي  لامتنا</t>
+  </si>
+  <si>
+    <t>تحركات البقاع تجديده امثال ايلي حبيقه وان تدخل اليبيوتنا وجه  الحضاره والسلام فنحنعندنا عيد برباره والدماءالملطخه صبرا وشاتيلا تجف”وكتب مراسل  “النهار النبطيهان المقاومه الاسلاميه احيتجبشيت ذكري اربعين شهداء مجزرهمكه حضور  وفد الجمهوريهالاسلاميه الايرانيه قوامه السيد محمدهاشمي والشيخ فلاخي والمستشارانسفاره ايران  بيروت السيدانمحمد ورحمتي وعلماء وجمهور
+  تحركات البقاع تجديده امثال ايلي حبيقه وان تدخل الى بيوتنا وجه  الحضاره والسلام فنحن عندنا عيد برباره والدماء الملطخه صبرا وشاتيلا تجف وكتب مراسل  النهار النبطيه ان المقاومه الاسلاميه احيت جبشيت ذكرى اربعين شهداء مجزره مكه حضور  وفد الجمهوريه الاسلاميه الايرانيه قوامه السيد محمد هاشمي والشيخ فلاخي والمستشار ان سفاره ايران  بيروت السيدان محمد ورحمتي وعلماء وجمهور</t>
+  </si>
+  <si>
+    <t>البلدين وقعا ايار الماضي اتفاقانغطيا سنويا تقدم بموجبه ايران اليسوريا  مليون طن النقط مجانامساهمه المجهود الحربي السوريضد اسرائيل تبيعها مليوني  طنبالسعر حددته منظمه البلدانالمصدره للنقط اوبيكالتتمه الصفحه ماسؤات تابلسلمجزره مخيمي  صبرا وشاتيلا
+  البلدين وقعا ايار الماضي اتفاق ان غطيا سنويا تقدم بموجبه ايران الى سوريا  مليون طن النفط مجانا مساهمه المجهود الحربي السوري ضد اسرائيل تبيعها مليوني  طن بالسعر حددته منظمه البلدان المصدره للنفط اوبيك التتمه الصفحه ماسؤات تابلس لمجزره مخيمي  صبرا وشاتيلا</t>
+  </si>
+  <si>
+    <t>ودعت الي مزيد اليفظهوالوحده اطراف الصف الوطنيوالاسلامي لتفويت الفرصه العوالصميوني  وعملاثه الوصول اليغايتهم تفتيت الصفوفواستنكر الامين العام التجمععكار السيد وجيهالبعريني  محاوله اغتيال البزري وصبراءودعا الي توحيد القوي الوطنيهوالموطه لمواجهه الهجمهالشرسه  تمدف الي تقجير الرموزالسفاره الادرانيهالذكري الخامسه لمجزره صبراوشاتيلاء دعت تنظيمات  لبنانيهوفلسطينيه الي انهاء هربالمخيمات ومواصله الكفاح المسلحضد اسرائيل
+  ودعت الى مزيد اليقظه والوحده اطراف الصف الوطني والاسلامي لتفويت الفرصه العدو الصهيوني  وعملائه الوصول الى غايتهم تفتيت الصفوف واستنكر الامين العام التجمع عكار السيد وجيه البعريني  محاوله اغتيال البزري وصبرا ودعا الى توحيد القوى الوطنيه والمواظبه لمواجهه الهجمه الشرسه  تهدف الى تفجير الرموز السفاره الاردنيه الذكرى الخامسه لمجزره صبرا وشاتيلا دعت تنظيمات  لبنانيه وفلسطينيه الى انهاء حرب المخيمات ومواصله الكفاح المسلح ضد اسرائيل</t>
+  </si>
+  <si>
+    <t>الصفحهالسفاره الايائيه احيتشاتيلاذكري المجزره واحدات مكهذكري اربعين شهداء مجزرهمكه والذكري  الخامسه لمجزره صبراوشاتيلاء اقامت سفاره جمهوريه ايرانالاسلاميه مهرجانا خطابيا مخيموفي  معلومات وزعتها السفاره انابناء المخيم استقيلوا اركانهابمسيره ترحيب رفعت شعاراتوهتافات  ايران ايرانفكوا عنا الحصار
+  الصفحه السفاره الايائيه احيت شاتيلا ذكرى المجزره واحداث مكه ذكرى اربعين شهداء مجزره مكه والذكرى  الخامسه لمجزره صبرا وشاتيلا اقامت سفاره جمهوريه ايران الاسلاميه مهرجانا خطابيا مخيم وفي  معلومات وزعتها السفاره ان ابناء المخيم استقبلوا اركانها بمسيره ترحيب رفعت شعارات وهتافات  ايران ايران فكوا عنا الحصار</t>
+  </si>
+  <si>
+    <t>الذكرك خاصسه للجزيه صفا وهاتلاتنيات يجب انياء حرب الاتالذكري الخامسه  لمجزره صبراوشاتيلا اقيمت ندوات ومهرجاناتالمخيمات الفلسطينيه وصدرت بياناتنددت بالمجزره وحضت  تنقيمبادره رئيس حركه امل الوزير نبيهبري لانهاء حرب المخيمات
+  الذكرى الخامسه للجزيه صفا وهاتلاتنيات يجب انياء حزب الله الذكرى الخامسه  لمجزره صبرا وشاتيلا اقيمت ندوات ومهرجانات المخيمات الفلسطينيه وصدرت بيانات نددت بالمجزره وحضت  نقي مبادره رئيس حركه امل الوزير نبيه بري لانهاء حرب المخيمات</t>
+  </si>
+  <si>
+    <t>اصدرت حركه فتح اقليم لبنانبيانا ذكري مجزره صبرا وشاتيلاءاكدت ان  هول الجريمه وبشاعهالمجزره جعلانا نؤمن ايمانا راسخابضروره ان نمتلك وساكل  الدفاعالنفس لئلا نسحق تحت اقدامالمجرمين يقيمون وزنا للقانونللاخلاق
+  اصدرت حركه فتح اقليم لبنان بيانا ذكرى مجزره صبرا وشاتيلا اكدت ان  هول الجريمه وبشاعه المجزره جعلانا نؤمن ايمانا راسخا بضروره ان نمتلك وسائل  الدفاع النفس لئلا نسحق تحت اقدام المجرمين يقيمون وزنا للقانون للاخلاق</t>
+  </si>
+  <si>
+    <t>وعرض الشيخ عبد الله الحلاقالمحطات التاريخيه التي مرتالقضيه الفلسطينيه الي  ان حصلالاجتياح ومجزره صبرا وشاتيلا ولفتالي ان الحكام عروشهم والشعوبضريبه  الدم غاليا انيعلموا ان الدماء ستهز الارضتحتهم هزت الارض تحت  الصهاينهالقزاه جنوب لبنان
+  وعرض الشيخ عبد الله الحلاق المحطات التاريخيه التي مرت القضيه الفلسطينيه الى  ان حصل الاجتياح ومجزره صبرا وشاتيلا ولفت الى ان الحكام عروشهم والشعوب ضريبه  الدم غاليا ان يعلموا ان الدماء ستهز الارض تحتهم هزت الارض تحت  الصهاينه الغزاه جنوب لبنان</t>
+  </si>
+  <si>
+    <t>وقال الدكتور علي عمار ان مجزرهصبرا وشاتيلا “لم تكن الاولي  تاريخامتناء فالمجازر ارتكبت ضدالمسلمين البلدء بتواطر وبانفسنا وبتخاذل منا وتامرواعتبر  ان المقاومه الاسلاميه بالرد المباشر المؤامرهالكبري والمجزره المشؤومه
+  وقال الدكتور علي عمار ان مجزره صبرا وشاتيلا لم تكن الاولي  تاريخ امتنا فالمجازر ارتكبت ضد المسلمين البلد بتواطئ وبانفسنا وبتخاذل منا وتامر واعتبر  ان المقاومه الاسلاميه بالرد المباشر المؤامره الكبرى والمجزره المشؤومه</t>
+  </si>
+  <si>
+    <t>جه لو جيش لبتان الجنوبي دواصيرت افواج المقاومه اللبنائيهامل بيانا  اعلنت ان مجموعهالشهيد مصطفي غدار المقاومهالمؤمنه كمنث صباح اليوم ذكريمجزره  صبرا وشاتيلا ووفاه الامام زينالعابدين لدوريه مشاه تابعه لجيشالعميل لحد  طريق الرادارالقطاع الاوسط وامطرتهابالرمايات اسلحه خفيفه ومتوسطهوقذائف صاروفيه فسقطاقرادها قتيل  وجريحالقدس رويتره اعلن ناطقعسكري القوات الاسرائيليه قتلتمسلحين اثنين امس اشتباكطرف  الحزام الامني
+  جه لو جيش لبنان الجنوبي واصدرت افواج المقاومه اللبنانيه امل بيانا  اعلنت ان مجموعه الشهيد مصطفى غدار المقاومه المؤمنه كمنت صباح اليوم ذكرى مجزره  صبرا وشاتيلا ووفاه الامام زين العابدين لدوريه مشاه تابعه لجيش العميل لحد  طريق الرادار القطاع الاوسط وامطرتها بالرمايات اسلحه خفيفه ومتوسطه وقذائف صاروخيه فسقط افرادها قتيل  وجريح القدس رويترز اعلن ناطق عسكري القوات الاسرائيليه قتل مسلحين اثنين امس اشتباك طرف  الحزام الامني</t>
+  </si>
+  <si>
+    <t>اظهرتالصفوف الاسرائيليه بيروت اثناءمجزره صبرا وشاتيلا
+  اظهرت الصفوف الاسرائيليه بيروت اثناء مجزره صبرا وشاتيلا</t>
+  </si>
+  <si>
     <t>Distant_Evaluation</t>
   </si>
   <si>
@@ -622,6 +963,9 @@
   </si>
   <si>
     <t>Distant_Historical</t>
+  </si>
+  <si>
+    <t>Loaded_Language</t>
   </si>
   <si>
     <t>1982</t>
@@ -997,7 +1341,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C146"/>
+  <dimension ref="A1:C230"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1019,10 +1363,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
-        <v>156</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1030,10 +1374,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="C3" t="s">
-        <v>156</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1041,10 +1385,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>150</v>
+        <v>234</v>
       </c>
       <c r="C4" t="s">
-        <v>156</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1052,10 +1396,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="C5" t="s">
-        <v>156</v>
+        <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1063,10 +1407,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>150</v>
+        <v>234</v>
       </c>
       <c r="C6" t="s">
-        <v>156</v>
+        <v>241</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1074,10 +1418,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="C7" t="s">
-        <v>157</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1085,10 +1429,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C8" t="s">
-        <v>157</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1096,10 +1440,10 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C9" t="s">
-        <v>157</v>
+        <v>242</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1107,10 +1451,10 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>151</v>
+        <v>235</v>
       </c>
       <c r="C10" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1118,10 +1462,10 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="C11" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1129,10 +1473,10 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>152</v>
+        <v>236</v>
       </c>
       <c r="C12" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1140,10 +1484,10 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C13" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1151,10 +1495,10 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>152</v>
+        <v>236</v>
       </c>
       <c r="C14" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1162,10 +1506,10 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="C15" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1173,10 +1517,10 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>150</v>
+        <v>234</v>
       </c>
       <c r="C16" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1184,10 +1528,10 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="C17" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1195,10 +1539,10 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C18" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1206,10 +1550,10 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>150</v>
+        <v>234</v>
       </c>
       <c r="C19" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1217,10 +1561,10 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>153</v>
+        <v>237</v>
       </c>
       <c r="C20" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1228,10 +1572,10 @@
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>154</v>
+        <v>238</v>
       </c>
       <c r="C21" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1239,10 +1583,10 @@
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="C22" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1250,10 +1594,10 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="C23" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1261,10 +1605,10 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>154</v>
+        <v>238</v>
       </c>
       <c r="C24" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1272,10 +1616,10 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>151</v>
+        <v>235</v>
       </c>
       <c r="C25" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1283,10 +1627,10 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C26" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1294,10 +1638,10 @@
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="C27" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1305,10 +1649,10 @@
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>151</v>
+        <v>235</v>
       </c>
       <c r="C28" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1316,10 +1660,10 @@
         <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>154</v>
+        <v>238</v>
       </c>
       <c r="C29" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1327,10 +1671,10 @@
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C30" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1338,10 +1682,10 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>151</v>
+        <v>235</v>
       </c>
       <c r="C31" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1349,10 +1693,10 @@
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>154</v>
+        <v>238</v>
       </c>
       <c r="C32" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1360,10 +1704,10 @@
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>153</v>
+        <v>237</v>
       </c>
       <c r="C33" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1371,10 +1715,10 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>154</v>
+        <v>238</v>
       </c>
       <c r="C34" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1382,10 +1726,10 @@
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="C35" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1393,10 +1737,10 @@
         <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="C36" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1404,10 +1748,10 @@
         <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>151</v>
+        <v>235</v>
       </c>
       <c r="C37" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1415,10 +1759,10 @@
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>150</v>
+        <v>234</v>
       </c>
       <c r="C38" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1426,10 +1770,10 @@
         <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="C39" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1437,10 +1781,10 @@
         <v>41</v>
       </c>
       <c r="B40" t="s">
-        <v>155</v>
+        <v>239</v>
       </c>
       <c r="C40" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1448,10 +1792,10 @@
         <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="C41" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1459,10 +1803,10 @@
         <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>155</v>
+        <v>239</v>
       </c>
       <c r="C42" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1470,10 +1814,10 @@
         <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>155</v>
+        <v>239</v>
       </c>
       <c r="C43" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1481,10 +1825,10 @@
         <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="C44" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1492,10 +1836,10 @@
         <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C45" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1503,10 +1847,10 @@
         <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C46" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1514,10 +1858,10 @@
         <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="C47" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1525,10 +1869,10 @@
         <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C48" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1536,10 +1880,10 @@
         <v>50</v>
       </c>
       <c r="B49" t="s">
-        <v>150</v>
+        <v>234</v>
       </c>
       <c r="C49" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1547,10 +1891,10 @@
         <v>51</v>
       </c>
       <c r="B50" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C50" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1558,10 +1902,10 @@
         <v>52</v>
       </c>
       <c r="B51" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C51" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1569,10 +1913,10 @@
         <v>53</v>
       </c>
       <c r="B52" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C52" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1580,10 +1924,10 @@
         <v>54</v>
       </c>
       <c r="B53" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C53" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1591,10 +1935,10 @@
         <v>55</v>
       </c>
       <c r="B54" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C54" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1602,10 +1946,10 @@
         <v>56</v>
       </c>
       <c r="B55" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C55" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1613,10 +1957,10 @@
         <v>57</v>
       </c>
       <c r="B56" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C56" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1624,10 +1968,10 @@
         <v>58</v>
       </c>
       <c r="B57" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="C57" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1635,10 +1979,10 @@
         <v>59</v>
       </c>
       <c r="B58" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C58" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1646,10 +1990,10 @@
         <v>60</v>
       </c>
       <c r="B59" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="C59" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1657,10 +2001,10 @@
         <v>61</v>
       </c>
       <c r="B60" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="C60" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1668,10 +2012,10 @@
         <v>62</v>
       </c>
       <c r="B61" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C61" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1679,10 +2023,10 @@
         <v>63</v>
       </c>
       <c r="B62" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C62" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1690,10 +2034,10 @@
         <v>64</v>
       </c>
       <c r="B63" t="s">
-        <v>152</v>
+        <v>236</v>
       </c>
       <c r="C63" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1701,10 +2045,10 @@
         <v>65</v>
       </c>
       <c r="B64" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C64" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1712,10 +2056,10 @@
         <v>66</v>
       </c>
       <c r="B65" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="C65" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1723,10 +2067,10 @@
         <v>67</v>
       </c>
       <c r="B66" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C66" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1734,10 +2078,10 @@
         <v>68</v>
       </c>
       <c r="B67" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="C67" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1745,10 +2089,10 @@
         <v>69</v>
       </c>
       <c r="B68" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C68" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1756,10 +2100,10 @@
         <v>70</v>
       </c>
       <c r="B69" t="s">
-        <v>154</v>
+        <v>238</v>
       </c>
       <c r="C69" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1767,10 +2111,10 @@
         <v>71</v>
       </c>
       <c r="B70" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="C70" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1778,10 +2122,10 @@
         <v>72</v>
       </c>
       <c r="B71" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="C71" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1789,10 +2133,10 @@
         <v>73</v>
       </c>
       <c r="B72" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="C72" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1800,10 +2144,10 @@
         <v>74</v>
       </c>
       <c r="B73" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C73" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1811,10 +2155,10 @@
         <v>75</v>
       </c>
       <c r="B74" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="C74" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -1822,10 +2166,10 @@
         <v>76</v>
       </c>
       <c r="B75" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C75" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1833,10 +2177,10 @@
         <v>77</v>
       </c>
       <c r="B76" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C76" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -1844,10 +2188,10 @@
         <v>78</v>
       </c>
       <c r="B77" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="C77" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -1855,10 +2199,10 @@
         <v>79</v>
       </c>
       <c r="B78" t="s">
-        <v>154</v>
+        <v>238</v>
       </c>
       <c r="C78" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -1866,10 +2210,10 @@
         <v>80</v>
       </c>
       <c r="B79" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="C79" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -1877,10 +2221,10 @@
         <v>81</v>
       </c>
       <c r="B80" t="s">
-        <v>154</v>
+        <v>238</v>
       </c>
       <c r="C80" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -1888,10 +2232,10 @@
         <v>82</v>
       </c>
       <c r="B81" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C81" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1899,10 +2243,10 @@
         <v>83</v>
       </c>
       <c r="B82" t="s">
-        <v>152</v>
+        <v>236</v>
       </c>
       <c r="C82" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -1910,10 +2254,10 @@
         <v>84</v>
       </c>
       <c r="B83" t="s">
-        <v>151</v>
+        <v>235</v>
       </c>
       <c r="C83" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1921,10 +2265,10 @@
         <v>85</v>
       </c>
       <c r="B84" t="s">
-        <v>150</v>
+        <v>234</v>
       </c>
       <c r="C84" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -1932,10 +2276,10 @@
         <v>86</v>
       </c>
       <c r="B85" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C85" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -1943,10 +2287,10 @@
         <v>87</v>
       </c>
       <c r="B86" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C86" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -1954,10 +2298,10 @@
         <v>88</v>
       </c>
       <c r="B87" t="s">
-        <v>150</v>
+        <v>234</v>
       </c>
       <c r="C87" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -1965,10 +2309,10 @@
         <v>89</v>
       </c>
       <c r="B88" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C88" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -1976,10 +2320,10 @@
         <v>90</v>
       </c>
       <c r="B89" t="s">
-        <v>153</v>
+        <v>237</v>
       </c>
       <c r="C89" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -1987,10 +2331,10 @@
         <v>91</v>
       </c>
       <c r="B90" t="s">
-        <v>153</v>
+        <v>237</v>
       </c>
       <c r="C90" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -1998,10 +2342,10 @@
         <v>92</v>
       </c>
       <c r="B91" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C91" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -2009,10 +2353,10 @@
         <v>93</v>
       </c>
       <c r="B92" t="s">
-        <v>154</v>
+        <v>238</v>
       </c>
       <c r="C92" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -2020,10 +2364,10 @@
         <v>94</v>
       </c>
       <c r="B93" t="s">
-        <v>150</v>
+        <v>234</v>
       </c>
       <c r="C93" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -2031,10 +2375,10 @@
         <v>95</v>
       </c>
       <c r="B94" t="s">
-        <v>151</v>
+        <v>235</v>
       </c>
       <c r="C94" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -2042,10 +2386,10 @@
         <v>96</v>
       </c>
       <c r="B95" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C95" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -2053,10 +2397,10 @@
         <v>97</v>
       </c>
       <c r="B96" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C96" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -2064,10 +2408,10 @@
         <v>98</v>
       </c>
       <c r="B97" t="s">
-        <v>155</v>
+        <v>239</v>
       </c>
       <c r="C97" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -2075,10 +2419,10 @@
         <v>99</v>
       </c>
       <c r="B98" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="C98" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -2086,7 +2430,7 @@
         <v>100</v>
       </c>
       <c r="C99" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -2094,7 +2438,7 @@
         <v>101</v>
       </c>
       <c r="C100" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -2102,10 +2446,10 @@
         <v>102</v>
       </c>
       <c r="B101" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C101" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -2113,10 +2457,10 @@
         <v>103</v>
       </c>
       <c r="B102" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="C102" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -2124,10 +2468,10 @@
         <v>104</v>
       </c>
       <c r="B103" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C103" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -2135,10 +2479,10 @@
         <v>105</v>
       </c>
       <c r="B104" t="s">
-        <v>150</v>
+        <v>234</v>
       </c>
       <c r="C104" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -2146,10 +2490,10 @@
         <v>106</v>
       </c>
       <c r="B105" t="s">
-        <v>154</v>
+        <v>238</v>
       </c>
       <c r="C105" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -2157,10 +2501,10 @@
         <v>107</v>
       </c>
       <c r="B106" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="C106" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -2168,10 +2512,10 @@
         <v>108</v>
       </c>
       <c r="B107" t="s">
-        <v>154</v>
+        <v>238</v>
       </c>
       <c r="C107" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -2179,10 +2523,10 @@
         <v>109</v>
       </c>
       <c r="B108" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="C108" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -2190,10 +2534,10 @@
         <v>110</v>
       </c>
       <c r="B109" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="C109" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -2201,10 +2545,10 @@
         <v>111</v>
       </c>
       <c r="B110" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C110" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -2212,10 +2556,10 @@
         <v>112</v>
       </c>
       <c r="B111" t="s">
-        <v>154</v>
+        <v>238</v>
       </c>
       <c r="C111" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -2223,10 +2567,10 @@
         <v>113</v>
       </c>
       <c r="B112" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C112" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -2234,10 +2578,10 @@
         <v>114</v>
       </c>
       <c r="B113" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="C113" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -2245,10 +2589,10 @@
         <v>115</v>
       </c>
       <c r="B114" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="C114" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -2256,10 +2600,10 @@
         <v>116</v>
       </c>
       <c r="B115" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="C115" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -2267,10 +2611,10 @@
         <v>117</v>
       </c>
       <c r="B116" t="s">
-        <v>150</v>
+        <v>234</v>
       </c>
       <c r="C116" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -2278,10 +2622,10 @@
         <v>118</v>
       </c>
       <c r="B117" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C117" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -2289,10 +2633,10 @@
         <v>119</v>
       </c>
       <c r="B118" t="s">
-        <v>152</v>
+        <v>236</v>
       </c>
       <c r="C118" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -2300,10 +2644,10 @@
         <v>120</v>
       </c>
       <c r="B119" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C119" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -2311,10 +2655,10 @@
         <v>121</v>
       </c>
       <c r="B120" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C120" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -2322,10 +2666,10 @@
         <v>122</v>
       </c>
       <c r="B121" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C121" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -2333,10 +2677,10 @@
         <v>123</v>
       </c>
       <c r="B122" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C122" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -2344,10 +2688,10 @@
         <v>124</v>
       </c>
       <c r="B123" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C123" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -2355,7 +2699,7 @@
         <v>125</v>
       </c>
       <c r="C124" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -2363,10 +2707,10 @@
         <v>126</v>
       </c>
       <c r="B125" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="C125" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -2374,10 +2718,10 @@
         <v>127</v>
       </c>
       <c r="B126" t="s">
-        <v>154</v>
+        <v>238</v>
       </c>
       <c r="C126" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -2385,10 +2729,10 @@
         <v>128</v>
       </c>
       <c r="B127" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C127" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -2396,10 +2740,10 @@
         <v>129</v>
       </c>
       <c r="B128" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="C128" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -2407,10 +2751,10 @@
         <v>130</v>
       </c>
       <c r="B129" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C129" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -2418,10 +2762,10 @@
         <v>131</v>
       </c>
       <c r="B130" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C130" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -2429,10 +2773,10 @@
         <v>132</v>
       </c>
       <c r="B131" t="s">
-        <v>152</v>
+        <v>236</v>
       </c>
       <c r="C131" t="s">
-        <v>156</v>
+        <v>241</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -2440,10 +2784,10 @@
         <v>133</v>
       </c>
       <c r="B132" t="s">
-        <v>152</v>
+        <v>236</v>
       </c>
       <c r="C132" t="s">
-        <v>156</v>
+        <v>241</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -2451,10 +2795,10 @@
         <v>134</v>
       </c>
       <c r="B133" t="s">
-        <v>154</v>
+        <v>238</v>
       </c>
       <c r="C133" t="s">
-        <v>156</v>
+        <v>241</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -2462,10 +2806,10 @@
         <v>135</v>
       </c>
       <c r="B134" t="s">
-        <v>154</v>
+        <v>238</v>
       </c>
       <c r="C134" t="s">
-        <v>156</v>
+        <v>241</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -2473,10 +2817,10 @@
         <v>136</v>
       </c>
       <c r="B135" t="s">
-        <v>150</v>
+        <v>234</v>
       </c>
       <c r="C135" t="s">
-        <v>156</v>
+        <v>241</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -2484,10 +2828,10 @@
         <v>137</v>
       </c>
       <c r="B136" t="s">
-        <v>150</v>
+        <v>234</v>
       </c>
       <c r="C136" t="s">
-        <v>156</v>
+        <v>241</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -2495,10 +2839,10 @@
         <v>138</v>
       </c>
       <c r="B137" t="s">
-        <v>150</v>
+        <v>234</v>
       </c>
       <c r="C137" t="s">
-        <v>156</v>
+        <v>241</v>
       </c>
     </row>
     <row r="138" spans="1:3">
@@ -2506,10 +2850,10 @@
         <v>139</v>
       </c>
       <c r="B138" t="s">
-        <v>150</v>
+        <v>234</v>
       </c>
       <c r="C138" t="s">
-        <v>156</v>
+        <v>241</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -2517,7 +2861,7 @@
         <v>140</v>
       </c>
       <c r="C139" t="s">
-        <v>156</v>
+        <v>241</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -2525,10 +2869,10 @@
         <v>141</v>
       </c>
       <c r="B140" t="s">
-        <v>154</v>
+        <v>238</v>
       </c>
       <c r="C140" t="s">
-        <v>156</v>
+        <v>241</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -2536,10 +2880,10 @@
         <v>142</v>
       </c>
       <c r="B141" t="s">
-        <v>150</v>
+        <v>234</v>
       </c>
       <c r="C141" t="s">
-        <v>161</v>
+        <v>246</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -2547,10 +2891,10 @@
         <v>143</v>
       </c>
       <c r="B142" t="s">
-        <v>150</v>
+        <v>234</v>
       </c>
       <c r="C142" t="s">
-        <v>161</v>
+        <v>246</v>
       </c>
     </row>
     <row r="143" spans="1:3">
@@ -2558,10 +2902,10 @@
         <v>144</v>
       </c>
       <c r="B143" t="s">
-        <v>155</v>
+        <v>239</v>
       </c>
       <c r="C143" t="s">
-        <v>157</v>
+        <v>242</v>
       </c>
     </row>
     <row r="144" spans="1:3">
@@ -2569,10 +2913,10 @@
         <v>145</v>
       </c>
       <c r="B144" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C144" t="s">
-        <v>157</v>
+        <v>242</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -2580,10 +2924,10 @@
         <v>146</v>
       </c>
       <c r="B145" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C145" t="s">
-        <v>157</v>
+        <v>242</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -2591,10 +2935,934 @@
         <v>147</v>
       </c>
       <c r="B146" t="s">
+        <v>232</v>
+      </c>
+      <c r="C146" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" t="s">
         <v>148</v>
       </c>
-      <c r="C146" t="s">
+      <c r="B147" t="s">
+        <v>238</v>
+      </c>
+      <c r="C147" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148" t="s">
+        <v>149</v>
+      </c>
+      <c r="B148" t="s">
+        <v>238</v>
+      </c>
+      <c r="C148" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="A149" t="s">
+        <v>150</v>
+      </c>
+      <c r="B149" t="s">
+        <v>236</v>
+      </c>
+      <c r="C149" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="A150" t="s">
+        <v>151</v>
+      </c>
+      <c r="B150" t="s">
+        <v>232</v>
+      </c>
+      <c r="C150" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
+      <c r="A151" t="s">
+        <v>152</v>
+      </c>
+      <c r="B151" t="s">
+        <v>238</v>
+      </c>
+      <c r="C151" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
+      <c r="A152" t="s">
+        <v>153</v>
+      </c>
+      <c r="B152" t="s">
+        <v>232</v>
+      </c>
+      <c r="C152" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="A153" t="s">
+        <v>154</v>
+      </c>
+      <c r="B153" t="s">
+        <v>239</v>
+      </c>
+      <c r="C153" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3">
+      <c r="A154" t="s">
+        <v>155</v>
+      </c>
+      <c r="B154" t="s">
+        <v>232</v>
+      </c>
+      <c r="C154" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3">
+      <c r="A155" t="s">
+        <v>156</v>
+      </c>
+      <c r="B155" t="s">
+        <v>232</v>
+      </c>
+      <c r="C155" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
+      <c r="A156" t="s">
         <v>157</v>
+      </c>
+      <c r="B156" t="s">
+        <v>232</v>
+      </c>
+      <c r="C156" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3">
+      <c r="A157" t="s">
+        <v>158</v>
+      </c>
+      <c r="B157" t="s">
+        <v>235</v>
+      </c>
+      <c r="C157" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3">
+      <c r="A158" t="s">
+        <v>159</v>
+      </c>
+      <c r="B158" t="s">
+        <v>238</v>
+      </c>
+      <c r="C158" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3">
+      <c r="A159" t="s">
+        <v>160</v>
+      </c>
+      <c r="B159" t="s">
+        <v>232</v>
+      </c>
+      <c r="C159" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3">
+      <c r="A160" t="s">
+        <v>161</v>
+      </c>
+      <c r="B160" t="s">
+        <v>232</v>
+      </c>
+      <c r="C160" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3">
+      <c r="A161" t="s">
+        <v>162</v>
+      </c>
+      <c r="B161" t="s">
+        <v>238</v>
+      </c>
+      <c r="C161" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3">
+      <c r="A162" t="s">
+        <v>163</v>
+      </c>
+      <c r="B162" t="s">
+        <v>232</v>
+      </c>
+      <c r="C162" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3">
+      <c r="A163" t="s">
+        <v>164</v>
+      </c>
+      <c r="B163" t="s">
+        <v>238</v>
+      </c>
+      <c r="C163" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3">
+      <c r="A164" t="s">
+        <v>165</v>
+      </c>
+      <c r="B164" t="s">
+        <v>232</v>
+      </c>
+      <c r="C164" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3">
+      <c r="A165" t="s">
+        <v>166</v>
+      </c>
+      <c r="B165" t="s">
+        <v>232</v>
+      </c>
+      <c r="C165" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3">
+      <c r="A166" t="s">
+        <v>167</v>
+      </c>
+      <c r="B166" t="s">
+        <v>232</v>
+      </c>
+      <c r="C166" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3">
+      <c r="A167" t="s">
+        <v>168</v>
+      </c>
+      <c r="B167" t="s">
+        <v>239</v>
+      </c>
+      <c r="C167" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3">
+      <c r="A168" t="s">
+        <v>169</v>
+      </c>
+      <c r="B168" t="s">
+        <v>232</v>
+      </c>
+      <c r="C168" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3">
+      <c r="A169" t="s">
+        <v>170</v>
+      </c>
+      <c r="B169" t="s">
+        <v>233</v>
+      </c>
+      <c r="C169" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3">
+      <c r="A170" t="s">
+        <v>171</v>
+      </c>
+      <c r="B170" t="s">
+        <v>238</v>
+      </c>
+      <c r="C170" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3">
+      <c r="A171" t="s">
+        <v>172</v>
+      </c>
+      <c r="B171" t="s">
+        <v>233</v>
+      </c>
+      <c r="C171" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3">
+      <c r="A172" t="s">
+        <v>173</v>
+      </c>
+      <c r="B172" t="s">
+        <v>238</v>
+      </c>
+      <c r="C172" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3">
+      <c r="A173" t="s">
+        <v>174</v>
+      </c>
+      <c r="B173" t="s">
+        <v>236</v>
+      </c>
+      <c r="C173" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3">
+      <c r="A174" t="s">
+        <v>175</v>
+      </c>
+      <c r="B174" t="s">
+        <v>232</v>
+      </c>
+      <c r="C174" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3">
+      <c r="A175" t="s">
+        <v>176</v>
+      </c>
+      <c r="B175" t="s">
+        <v>232</v>
+      </c>
+      <c r="C175" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3">
+      <c r="A176" t="s">
+        <v>177</v>
+      </c>
+      <c r="B176" t="s">
+        <v>235</v>
+      </c>
+      <c r="C176" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3">
+      <c r="A177" t="s">
+        <v>178</v>
+      </c>
+      <c r="B177" t="s">
+        <v>232</v>
+      </c>
+      <c r="C177" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3">
+      <c r="A178" t="s">
+        <v>179</v>
+      </c>
+      <c r="B178" t="s">
+        <v>234</v>
+      </c>
+      <c r="C178" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3">
+      <c r="A179" t="s">
+        <v>180</v>
+      </c>
+      <c r="B179" t="s">
+        <v>238</v>
+      </c>
+      <c r="C179" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3">
+      <c r="A180" t="s">
+        <v>181</v>
+      </c>
+      <c r="B180" t="s">
+        <v>233</v>
+      </c>
+      <c r="C180" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3">
+      <c r="A181" t="s">
+        <v>182</v>
+      </c>
+      <c r="B181" t="s">
+        <v>238</v>
+      </c>
+      <c r="C181" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3">
+      <c r="A182" t="s">
+        <v>183</v>
+      </c>
+      <c r="B182" t="s">
+        <v>238</v>
+      </c>
+      <c r="C182" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3">
+      <c r="A183" t="s">
+        <v>184</v>
+      </c>
+      <c r="B183" t="s">
+        <v>232</v>
+      </c>
+      <c r="C183" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3">
+      <c r="A184" t="s">
+        <v>185</v>
+      </c>
+      <c r="B184" t="s">
+        <v>238</v>
+      </c>
+      <c r="C184" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3">
+      <c r="A185" t="s">
+        <v>186</v>
+      </c>
+      <c r="B185" t="s">
+        <v>232</v>
+      </c>
+      <c r="C185" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3">
+      <c r="A186" t="s">
+        <v>187</v>
+      </c>
+      <c r="B186" t="s">
+        <v>238</v>
+      </c>
+      <c r="C186" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3">
+      <c r="A187" t="s">
+        <v>188</v>
+      </c>
+      <c r="B187" t="s">
+        <v>233</v>
+      </c>
+      <c r="C187" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3">
+      <c r="A188" t="s">
+        <v>189</v>
+      </c>
+      <c r="B188" t="s">
+        <v>239</v>
+      </c>
+      <c r="C188" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3">
+      <c r="A189" t="s">
+        <v>190</v>
+      </c>
+      <c r="B189" t="s">
+        <v>232</v>
+      </c>
+      <c r="C189" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3">
+      <c r="A190" t="s">
+        <v>191</v>
+      </c>
+      <c r="B190" t="s">
+        <v>238</v>
+      </c>
+      <c r="C190" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3">
+      <c r="A191" t="s">
+        <v>192</v>
+      </c>
+      <c r="B191" t="s">
+        <v>233</v>
+      </c>
+      <c r="C191" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3">
+      <c r="A192" t="s">
+        <v>193</v>
+      </c>
+      <c r="B192" t="s">
+        <v>232</v>
+      </c>
+      <c r="C192" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3">
+      <c r="A193" t="s">
+        <v>194</v>
+      </c>
+      <c r="B193" t="s">
+        <v>238</v>
+      </c>
+      <c r="C193" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3">
+      <c r="A194" t="s">
+        <v>195</v>
+      </c>
+      <c r="B194" t="s">
+        <v>233</v>
+      </c>
+      <c r="C194" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3">
+      <c r="A195" t="s">
+        <v>196</v>
+      </c>
+      <c r="B195" t="s">
+        <v>232</v>
+      </c>
+      <c r="C195" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3">
+      <c r="A196" t="s">
+        <v>197</v>
+      </c>
+      <c r="B196" t="s">
+        <v>238</v>
+      </c>
+      <c r="C196" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3">
+      <c r="A197" t="s">
+        <v>198</v>
+      </c>
+      <c r="B197" t="s">
+        <v>233</v>
+      </c>
+      <c r="C197" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3">
+      <c r="A198" t="s">
+        <v>199</v>
+      </c>
+      <c r="B198" t="s">
+        <v>239</v>
+      </c>
+      <c r="C198" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3">
+      <c r="A199" t="s">
+        <v>200</v>
+      </c>
+      <c r="B199" t="s">
+        <v>239</v>
+      </c>
+      <c r="C199" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3">
+      <c r="A200" t="s">
+        <v>201</v>
+      </c>
+      <c r="B200" t="s">
+        <v>232</v>
+      </c>
+      <c r="C200" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3">
+      <c r="A201" t="s">
+        <v>202</v>
+      </c>
+      <c r="B201" t="s">
+        <v>233</v>
+      </c>
+      <c r="C201" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3">
+      <c r="A202" t="s">
+        <v>203</v>
+      </c>
+      <c r="B202" t="s">
+        <v>236</v>
+      </c>
+      <c r="C202" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3">
+      <c r="A203" t="s">
+        <v>204</v>
+      </c>
+      <c r="B203" t="s">
+        <v>236</v>
+      </c>
+      <c r="C203" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3">
+      <c r="A204" t="s">
+        <v>205</v>
+      </c>
+      <c r="B204" t="s">
+        <v>232</v>
+      </c>
+      <c r="C204" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3">
+      <c r="A205" t="s">
+        <v>206</v>
+      </c>
+      <c r="B205" t="s">
+        <v>238</v>
+      </c>
+      <c r="C205" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3">
+      <c r="A206" t="s">
+        <v>207</v>
+      </c>
+      <c r="B206" t="s">
+        <v>238</v>
+      </c>
+      <c r="C206" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3">
+      <c r="A207" t="s">
+        <v>208</v>
+      </c>
+      <c r="B207" t="s">
+        <v>232</v>
+      </c>
+      <c r="C207" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3">
+      <c r="A208" t="s">
+        <v>209</v>
+      </c>
+      <c r="B208" t="s">
+        <v>238</v>
+      </c>
+      <c r="C208" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3">
+      <c r="A209" t="s">
+        <v>210</v>
+      </c>
+      <c r="B209" t="s">
+        <v>232</v>
+      </c>
+      <c r="C209" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3">
+      <c r="A210" t="s">
+        <v>211</v>
+      </c>
+      <c r="B210" t="s">
+        <v>238</v>
+      </c>
+      <c r="C210" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3">
+      <c r="A211" t="s">
+        <v>212</v>
+      </c>
+      <c r="B211" t="s">
+        <v>233</v>
+      </c>
+      <c r="C211" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3">
+      <c r="A212" t="s">
+        <v>213</v>
+      </c>
+      <c r="B212" t="s">
+        <v>232</v>
+      </c>
+      <c r="C212" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3">
+      <c r="A213" t="s">
+        <v>214</v>
+      </c>
+      <c r="B213" t="s">
+        <v>238</v>
+      </c>
+      <c r="C213" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3">
+      <c r="A214" t="s">
+        <v>215</v>
+      </c>
+      <c r="B214" t="s">
+        <v>233</v>
+      </c>
+      <c r="C214" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3">
+      <c r="A215" t="s">
+        <v>216</v>
+      </c>
+      <c r="B215" t="s">
+        <v>232</v>
+      </c>
+      <c r="C215" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3">
+      <c r="A216" t="s">
+        <v>217</v>
+      </c>
+      <c r="B216" t="s">
+        <v>233</v>
+      </c>
+      <c r="C216" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3">
+      <c r="A217" t="s">
+        <v>218</v>
+      </c>
+      <c r="B217" t="s">
+        <v>240</v>
+      </c>
+      <c r="C217" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3">
+      <c r="A218" t="s">
+        <v>219</v>
+      </c>
+      <c r="B218" t="s">
+        <v>232</v>
+      </c>
+      <c r="C218" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3">
+      <c r="A219" t="s">
+        <v>220</v>
+      </c>
+      <c r="B219" t="s">
+        <v>232</v>
+      </c>
+      <c r="C219" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3">
+      <c r="A220" t="s">
+        <v>221</v>
+      </c>
+      <c r="B220" t="s">
+        <v>238</v>
+      </c>
+      <c r="C220" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3">
+      <c r="A221" t="s">
+        <v>222</v>
+      </c>
+      <c r="B221" t="s">
+        <v>238</v>
+      </c>
+      <c r="C221" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3">
+      <c r="A222" t="s">
+        <v>223</v>
+      </c>
+      <c r="B222" t="s">
+        <v>239</v>
+      </c>
+      <c r="C222" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3">
+      <c r="A223" t="s">
+        <v>224</v>
+      </c>
+      <c r="B223" t="s">
+        <v>238</v>
+      </c>
+      <c r="C223" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3">
+      <c r="A224" t="s">
+        <v>225</v>
+      </c>
+      <c r="B224" t="s">
+        <v>238</v>
+      </c>
+      <c r="C224" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3">
+      <c r="A225" t="s">
+        <v>226</v>
+      </c>
+      <c r="B225" t="s">
+        <v>238</v>
+      </c>
+      <c r="C225" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3">
+      <c r="A226" t="s">
+        <v>227</v>
+      </c>
+      <c r="B226" t="s">
+        <v>232</v>
+      </c>
+      <c r="C226" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3">
+      <c r="A227" t="s">
+        <v>228</v>
+      </c>
+      <c r="B227" t="s">
+        <v>233</v>
+      </c>
+      <c r="C227" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3">
+      <c r="A228" t="s">
+        <v>229</v>
+      </c>
+      <c r="B228" t="s">
+        <v>239</v>
+      </c>
+      <c r="C228" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3">
+      <c r="A229" t="s">
+        <v>230</v>
+      </c>
+      <c r="B229" t="s">
+        <v>236</v>
+      </c>
+      <c r="C229" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3">
+      <c r="A230" t="s">
+        <v>231</v>
+      </c>
+      <c r="B230" t="s">
+        <v>232</v>
+      </c>
+      <c r="C230" t="s">
+        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>